<commit_message>
More work to $ADSK model
</commit_message>
<xml_diff>
--- a/$ADSK.xlsx
+++ b/$ADSK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AADDDC-38D2-47F3-B263-7474DB19095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456794CE-9D31-49CB-9F25-F9ED131C077B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>$ADSK</t>
   </si>
@@ -148,15 +148,6 @@
     <t>Q123</t>
   </si>
   <si>
-    <t>Q122</t>
-  </si>
-  <si>
-    <t>Q22</t>
-  </si>
-  <si>
-    <t>Q322</t>
-  </si>
-  <si>
     <t>Subscription Revenue</t>
   </si>
   <si>
@@ -323,6 +314,69 @@
   </si>
   <si>
     <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Cashflow</t>
+  </si>
+  <si>
+    <t>CFFO</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>FCF</t>
+  </si>
+  <si>
+    <t>FCF per Share</t>
+  </si>
+  <si>
+    <t>Price to FCF</t>
+  </si>
+  <si>
+    <t>FCF TTM</t>
+  </si>
+  <si>
+    <t>Q125</t>
+  </si>
+  <si>
+    <t>Q225</t>
+  </si>
+  <si>
+    <t>Q424</t>
+  </si>
+  <si>
+    <t>Q324</t>
+  </si>
+  <si>
+    <t>FY18</t>
+  </si>
+  <si>
+    <t>FY19</t>
+  </si>
+  <si>
+    <t>FY20</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY23</t>
+  </si>
+  <si>
+    <t>FY24</t>
+  </si>
+  <si>
+    <t>FY25</t>
+  </si>
+  <si>
+    <t>FY26</t>
+  </si>
+  <si>
+    <t>FY27</t>
   </si>
 </sst>
 </file>
@@ -332,7 +386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="170" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +442,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -509,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -597,6 +657,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -982,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BFD011-71B1-4504-B133-A0FB7BFF1926}">
   <dimension ref="B2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1426,10 +1492,10 @@
       <c r="B30" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="44"/>
       <c r="G30" s="15"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
@@ -1501,8 +1567,11 @@
       <c r="B35" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
+      <c r="C35" s="41">
+        <f>+C8/SUM('Financial Model'!I7:L7)</f>
+        <v>11.954232558139534</v>
+      </c>
+      <c r="D35" s="42"/>
       <c r="G35" s="15"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
@@ -1517,8 +1586,11 @@
       <c r="B36" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
+      <c r="C36" s="41">
+        <f>+C6/SUM('Financial Model'!I22:L22)</f>
+        <v>65.277899355462978</v>
+      </c>
+      <c r="D36" s="42"/>
       <c r="G36" s="15"/>
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
@@ -1613,393 +1685,1258 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C30:D30" r:id="rId1" display="Link" xr:uid="{136B0ED8-5FD6-4628-BBD0-474E201794EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962F6E9D-1442-4F5B-A570-7043CF769B1D}">
-  <dimension ref="B1:L75"/>
+  <dimension ref="B1:Z86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B80" sqref="B80"/>
+      <selection pane="bottomRight" activeCell="U85" sqref="U85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="9.140625" style="2"/>
     <col min="12" max="12" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:26" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="2:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="25"/>
+      <c r="E2" s="30">
+        <v>44865</v>
+      </c>
+      <c r="F2" s="30">
+        <v>44926</v>
+      </c>
+      <c r="G2" s="30">
+        <v>45046</v>
+      </c>
       <c r="H2" s="30">
         <v>45138</v>
       </c>
+      <c r="I2" s="30">
+        <v>45230</v>
+      </c>
+      <c r="J2" s="30">
+        <v>45291</v>
+      </c>
+      <c r="K2" s="30">
+        <v>45412</v>
+      </c>
       <c r="L2" s="30">
         <v>45504</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U2" s="30">
+        <v>44592</v>
+      </c>
+      <c r="V2" s="30">
+        <v>44957</v>
+      </c>
+      <c r="W2" s="30">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
+      <c r="I3" s="28">
+        <v>45264</v>
+      </c>
+      <c r="J3" s="28">
+        <v>45351</v>
+      </c>
+      <c r="K3" s="28">
+        <v>45453</v>
+      </c>
       <c r="L3" s="28">
         <v>45538</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="28">
+        <f>+J3</f>
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="31" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="E4" s="32">
+        <v>1188</v>
+      </c>
+      <c r="G4" s="32">
+        <v>1193</v>
       </c>
       <c r="H4" s="32">
         <v>1270</v>
       </c>
+      <c r="I4" s="32">
+        <v>1314</v>
+      </c>
+      <c r="J4" s="32">
+        <f>+W4-SUM(G4:I4)</f>
+        <v>1339</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1330</v>
+      </c>
       <c r="L4" s="32">
         <v>1408</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U4" s="32">
+        <v>4060</v>
+      </c>
+      <c r="V4" s="32">
+        <v>4651</v>
+      </c>
+      <c r="W4" s="32">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="31" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="E5" s="32">
+        <v>16</v>
+      </c>
+      <c r="G5" s="32">
+        <v>14</v>
       </c>
       <c r="H5" s="32">
         <v>14</v>
       </c>
+      <c r="I5" s="32">
+        <v>12</v>
+      </c>
+      <c r="J5" s="32">
+        <f>+W5-SUM(G5:I5)</f>
+        <v>14</v>
+      </c>
+      <c r="K5" s="32">
+        <v>11</v>
+      </c>
       <c r="L5" s="32">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U5" s="32">
+        <v>76</v>
+      </c>
+      <c r="V5" s="32">
+        <v>65</v>
+      </c>
+      <c r="W5" s="32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="31" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="E6" s="32">
+        <v>76</v>
+      </c>
+      <c r="G6" s="32">
+        <v>62</v>
       </c>
       <c r="H6" s="32">
         <v>61</v>
       </c>
+      <c r="I6" s="32">
+        <v>88</v>
+      </c>
+      <c r="J6" s="32">
+        <f>+W6-SUM(G6:I6)</f>
+        <v>116</v>
+      </c>
+      <c r="K6" s="32">
+        <v>76</v>
+      </c>
       <c r="L6" s="32">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U6" s="32">
+        <v>250</v>
+      </c>
+      <c r="V6" s="32">
+        <v>289</v>
+      </c>
+      <c r="W6" s="32">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="33" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C7" s="33">
+        <f t="shared" ref="C7:F7" si="0">+SUM(C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+      <c r="F7" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <f>+SUM(G4:G6)</f>
+        <v>1269</v>
       </c>
       <c r="H7" s="33">
         <f>+SUM(H4:H6)</f>
         <v>1345</v>
       </c>
+      <c r="I7" s="33">
+        <f>+SUM(I4:I6)</f>
+        <v>1414</v>
+      </c>
+      <c r="J7" s="33">
+        <f t="shared" ref="J7" si="1">+SUM(J4:J6)</f>
+        <v>1469</v>
+      </c>
+      <c r="K7" s="33">
+        <f>+SUM(K4:K6)</f>
+        <v>1417</v>
+      </c>
       <c r="L7" s="33">
         <f>+SUM(L4:L6)</f>
         <v>1505</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U7" s="33">
+        <f t="shared" ref="U7:W7" si="2">+SUM(U4:U6)</f>
+        <v>4386</v>
+      </c>
+      <c r="V7" s="33">
+        <f t="shared" si="2"/>
+        <v>5005</v>
+      </c>
+      <c r="W7" s="33">
+        <f t="shared" si="2"/>
+        <v>5497</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="E8" s="32">
+        <v>86</v>
+      </c>
+      <c r="G8" s="32">
+        <v>96</v>
       </c>
       <c r="H8" s="32">
         <v>95</v>
       </c>
+      <c r="I8" s="32">
+        <v>94</v>
+      </c>
+      <c r="J8" s="32">
+        <f>+W8-SUM(G8:I8)</f>
+        <v>96</v>
+      </c>
+      <c r="K8" s="32">
+        <v>100</v>
+      </c>
       <c r="L8" s="32">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U8" s="32">
+        <v>299</v>
+      </c>
+      <c r="V8" s="32">
+        <v>343</v>
+      </c>
+      <c r="W8" s="32">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="31" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="E9" s="32">
+        <v>19</v>
+      </c>
+      <c r="G9" s="32">
+        <v>20</v>
       </c>
       <c r="H9" s="32">
         <v>21</v>
       </c>
+      <c r="I9" s="32">
+        <v>21</v>
+      </c>
+      <c r="J9" s="32">
+        <f>+W9-SUM(G9:I9)</f>
+        <v>20</v>
+      </c>
+      <c r="K9" s="32">
+        <v>20</v>
+      </c>
       <c r="L9" s="32">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U9" s="32">
+        <v>67</v>
+      </c>
+      <c r="V9" s="32">
+        <v>79</v>
+      </c>
+      <c r="W9" s="32">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="32">
+        <v>15</v>
+      </c>
+      <c r="G10" s="32">
+        <v>11</v>
       </c>
       <c r="H10" s="32">
         <v>11</v>
       </c>
+      <c r="I10" s="32">
+        <v>12</v>
+      </c>
+      <c r="J10" s="32">
+        <f>+W10-SUM(G10:I10)</f>
+        <v>14</v>
+      </c>
+      <c r="K10" s="32">
+        <v>17</v>
+      </c>
       <c r="L10" s="32">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U10" s="32">
+        <v>52</v>
+      </c>
+      <c r="V10" s="32">
+        <v>58</v>
+      </c>
+      <c r="W10" s="32">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C11" s="32">
+        <f t="shared" ref="C11:F11" si="3">SUM(C8:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="F11" s="32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
+        <f>SUM(G8:G10)</f>
+        <v>127</v>
       </c>
       <c r="H11" s="32">
         <f>SUM(H8:H10)</f>
         <v>127</v>
       </c>
+      <c r="I11" s="32">
+        <f>SUM(I8:I10)</f>
+        <v>127</v>
+      </c>
+      <c r="J11" s="32">
+        <f t="shared" ref="J11" si="4">SUM(J8:J10)</f>
+        <v>130</v>
+      </c>
+      <c r="K11" s="32">
+        <f>SUM(K8:K10)</f>
+        <v>137</v>
+      </c>
       <c r="L11" s="32">
         <f>SUM(L8:L10)</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U11" s="32">
+        <f t="shared" ref="U11:W11" si="5">SUM(U8:U10)</f>
+        <v>418</v>
+      </c>
+      <c r="V11" s="32">
+        <f t="shared" si="5"/>
+        <v>480</v>
+      </c>
+      <c r="W11" s="32">
+        <f t="shared" si="5"/>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="33">
+        <f t="shared" ref="C12:F12" si="6">+C7-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <f t="shared" si="6"/>
+        <v>1160</v>
+      </c>
+      <c r="F12" s="33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <f>+G7-G11</f>
+        <v>1142</v>
       </c>
       <c r="H12" s="33">
+        <f>+H7-H11</f>
         <v>1218</v>
+      </c>
+      <c r="I12" s="33">
+        <f>+I7-I11</f>
+        <v>1287</v>
+      </c>
+      <c r="J12" s="33">
+        <f t="shared" ref="J12" si="7">+J7-J11</f>
+        <v>1339</v>
+      </c>
+      <c r="K12" s="33">
+        <f>+K7-K11</f>
+        <v>1280</v>
       </c>
       <c r="L12" s="33">
         <f>+L7-L11</f>
         <v>1365</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U12" s="33">
+        <f t="shared" ref="U12:W12" si="8">+U7-U11</f>
+        <v>3968</v>
+      </c>
+      <c r="V12" s="33">
+        <f t="shared" si="8"/>
+        <v>4525</v>
+      </c>
+      <c r="W12" s="33">
+        <f t="shared" si="8"/>
+        <v>4986</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E13" s="2">
+        <v>454</v>
+      </c>
+      <c r="G13" s="2">
+        <v>456</v>
       </c>
       <c r="H13" s="2">
         <v>449</v>
       </c>
+      <c r="I13" s="2">
+        <v>439</v>
+      </c>
+      <c r="J13" s="32">
+        <f>+W13-SUM(G13:I13)</f>
+        <v>479</v>
+      </c>
+      <c r="K13" s="2">
+        <v>469</v>
+      </c>
       <c r="L13" s="2">
         <v>480</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U13" s="2">
+        <v>1623</v>
+      </c>
+      <c r="V13" s="2">
+        <v>1745</v>
+      </c>
+      <c r="W13" s="2">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="E14" s="2">
+        <v>311</v>
+      </c>
+      <c r="G14" s="2">
+        <v>327</v>
       </c>
       <c r="H14" s="2">
         <v>355</v>
       </c>
+      <c r="I14" s="2">
+        <v>339</v>
+      </c>
+      <c r="J14" s="32">
+        <f>+W14-SUM(G14:I14)</f>
+        <v>352</v>
+      </c>
+      <c r="K14" s="2">
+        <v>346</v>
+      </c>
       <c r="L14" s="2">
         <v>368</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U14" s="2">
+        <v>1115</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1219</v>
+      </c>
+      <c r="W14" s="2">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="E15" s="2">
+        <v>129</v>
+      </c>
+      <c r="G15" s="2">
+        <v>132</v>
       </c>
       <c r="H15" s="2">
         <v>141</v>
       </c>
+      <c r="I15" s="2">
+        <v>165</v>
+      </c>
+      <c r="J15" s="32">
+        <f>+W15-SUM(G15:I15)</f>
+        <v>182</v>
+      </c>
+      <c r="K15" s="2">
+        <v>155</v>
+      </c>
       <c r="L15" s="2">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U15" s="2">
+        <v>572</v>
+      </c>
+      <c r="V15" s="2">
+        <v>532</v>
+      </c>
+      <c r="W15" s="2">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>10</v>
       </c>
       <c r="H16" s="2">
         <v>11</v>
       </c>
+      <c r="I16" s="2">
+        <v>10</v>
+      </c>
+      <c r="J16" s="32">
+        <f>+W16-SUM(G16:I16)</f>
+        <v>11</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11</v>
+      </c>
       <c r="L16" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U16" s="2">
+        <v>40</v>
+      </c>
+      <c r="V16" s="2">
+        <v>40</v>
+      </c>
+      <c r="W16" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="C17" s="33">
+        <f t="shared" ref="C17:F17" si="9">+C12-SUM(C13:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <f t="shared" si="9"/>
+        <v>256</v>
+      </c>
+      <c r="F17" s="33">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <f>+G12-SUM(G13:G16)</f>
+        <v>217</v>
       </c>
       <c r="H17" s="33">
         <f>+H12-SUM(H13:H16)</f>
         <v>262</v>
       </c>
+      <c r="I17" s="33">
+        <f>+I12-SUM(I13:I16)</f>
+        <v>334</v>
+      </c>
+      <c r="J17" s="33">
+        <f t="shared" ref="J17" si="10">+J12-SUM(J13:J16)</f>
+        <v>315</v>
+      </c>
+      <c r="K17" s="33">
+        <f>+K12-SUM(K13:K16)</f>
+        <v>299</v>
+      </c>
       <c r="L17" s="33">
         <f>+L12-SUM(L13:L16)</f>
         <v>343</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U17" s="33">
+        <f t="shared" ref="U17:W17" si="11">+U12-SUM(U13:U16)</f>
+        <v>618</v>
+      </c>
+      <c r="V17" s="33">
+        <f t="shared" si="11"/>
+        <v>989</v>
+      </c>
+      <c r="W17" s="33">
+        <f t="shared" si="11"/>
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-14</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
       </c>
       <c r="H18" s="2">
         <v>-4</v>
       </c>
+      <c r="I18" s="2">
+        <v>-14</v>
+      </c>
+      <c r="J18" s="32">
+        <f>+W18-SUM(G18:I18)</f>
+        <v>22</v>
+      </c>
+      <c r="K18" s="2">
+        <v>10</v>
+      </c>
       <c r="L18" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U18" s="2">
+        <v>-53</v>
+      </c>
+      <c r="V18" s="2">
+        <v>-43</v>
+      </c>
+      <c r="W18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="C19" s="32">
+        <f t="shared" ref="C19:F19" si="12">+C17+C18</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="32">
+        <f t="shared" si="12"/>
+        <v>242</v>
+      </c>
+      <c r="F19" s="32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <f>+G17+G18</f>
+        <v>221</v>
       </c>
       <c r="H19" s="32">
         <f>+H17+H18</f>
         <v>258</v>
       </c>
+      <c r="I19" s="32">
+        <f>+I17+I18</f>
+        <v>320</v>
+      </c>
+      <c r="J19" s="32">
+        <f t="shared" ref="J19" si="13">+J17+J18</f>
+        <v>337</v>
+      </c>
+      <c r="K19" s="32">
+        <f>+K17+K18</f>
+        <v>309</v>
+      </c>
       <c r="L19" s="32">
         <f>+L17+L18</f>
         <v>352</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U19" s="32">
+        <f t="shared" ref="U19:W19" si="14">+U17+U18</f>
+        <v>565</v>
+      </c>
+      <c r="V19" s="32">
+        <f t="shared" si="14"/>
+        <v>946</v>
+      </c>
+      <c r="W19" s="32">
+        <f t="shared" si="14"/>
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44</v>
+      </c>
+      <c r="G20" s="2">
+        <v>60</v>
       </c>
       <c r="H20" s="2">
         <v>36</v>
       </c>
+      <c r="I20" s="2">
+        <v>79</v>
+      </c>
+      <c r="J20" s="32">
+        <f>+W20-SUM(G20:I20)</f>
+        <v>55</v>
+      </c>
+      <c r="K20" s="2">
+        <v>57</v>
+      </c>
       <c r="L20" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U20" s="2">
+        <v>68</v>
+      </c>
+      <c r="V20" s="2">
+        <v>123</v>
+      </c>
+      <c r="W20" s="2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="C21" s="33">
+        <f t="shared" ref="C21:F21" si="15">+C19-C20</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <f t="shared" si="15"/>
+        <v>198</v>
+      </c>
+      <c r="F21" s="33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <f>+G19-G20</f>
+        <v>161</v>
       </c>
       <c r="H21" s="33">
         <f>+H19-H20</f>
         <v>222</v>
       </c>
+      <c r="I21" s="33">
+        <f>+I19-I20</f>
+        <v>241</v>
+      </c>
+      <c r="J21" s="33">
+        <f t="shared" ref="J21" si="16">+J19-J20</f>
+        <v>282</v>
+      </c>
+      <c r="K21" s="33">
+        <f>+K19-K20</f>
+        <v>252</v>
+      </c>
       <c r="L21" s="33">
         <f>+L19-L20</f>
         <v>282</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U21" s="33">
+        <f t="shared" ref="U21:W21" si="17">+U19-U20</f>
+        <v>497</v>
+      </c>
+      <c r="V21" s="33">
+        <f t="shared" si="17"/>
+        <v>823</v>
+      </c>
+      <c r="W21" s="33">
+        <f t="shared" si="17"/>
+        <v>906</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="34" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="E22" s="34">
+        <f>+E21/E23</f>
+        <v>0.9124423963133641</v>
+      </c>
+      <c r="G22" s="34">
+        <f>+G21/G23</f>
+        <v>0.74883720930232556</v>
       </c>
       <c r="H22" s="34">
         <f>+H21/H23</f>
         <v>1.0373831775700935</v>
       </c>
+      <c r="I22" s="34">
+        <f>+I21/I23</f>
+        <v>1.1261682242990654</v>
+      </c>
+      <c r="J22" s="34">
+        <f>+J21/J23</f>
+        <v>1.3177570093457944</v>
+      </c>
+      <c r="K22" s="34">
+        <f>+K21/K23</f>
+        <v>1.172093023255814</v>
+      </c>
       <c r="L22" s="34">
         <f>+L21/L23</f>
         <v>1.3055555555555556</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="U22" s="34">
+        <f>+U21/U23</f>
+        <v>2.2590909090909093</v>
+      </c>
+      <c r="V22" s="34">
+        <f>+V21/V23</f>
+        <v>3.8101851851851851</v>
+      </c>
+      <c r="W22" s="34">
+        <f>+W21/W23</f>
+        <v>4.2336448598130838</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E23" s="2">
+        <v>217</v>
+      </c>
+      <c r="G23" s="2">
+        <v>215</v>
+      </c>
       <c r="H23" s="2">
         <v>214</v>
       </c>
+      <c r="I23" s="2">
+        <v>214</v>
+      </c>
+      <c r="J23" s="2">
+        <f>+W23</f>
+        <v>214</v>
+      </c>
+      <c r="K23" s="2">
+        <v>215</v>
+      </c>
       <c r="L23" s="2">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U23" s="2">
+        <v>220</v>
+      </c>
+      <c r="V23" s="2">
+        <v>216</v>
+      </c>
+      <c r="W23" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="36" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="E25" s="36">
+        <f>+E12/E7</f>
+        <v>0.90625</v>
+      </c>
+      <c r="G25" s="36">
+        <f>+G12/G7</f>
+        <v>0.89992119779353819</v>
       </c>
       <c r="H25" s="36">
         <f>+H12/H7</f>
         <v>0.90557620817843865</v>
       </c>
+      <c r="I25" s="36">
+        <f>+I12/I7</f>
+        <v>0.91018387553041014</v>
+      </c>
+      <c r="J25" s="36">
+        <f>+J12/J7</f>
+        <v>0.91150442477876104</v>
+      </c>
+      <c r="K25" s="36">
+        <f>+K12/K7</f>
+        <v>0.90331686661961896</v>
+      </c>
       <c r="L25" s="36">
         <f>+L12/L7</f>
         <v>0.90697674418604646</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U25" s="36">
+        <f>+U12/U7</f>
+        <v>0.90469676242590058</v>
+      </c>
+      <c r="V25" s="36">
+        <f>+V12/V7</f>
+        <v>0.90409590409590412</v>
+      </c>
+      <c r="W25" s="36">
+        <f>+W12/W7</f>
+        <v>0.90704020374749861</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="36" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="E26" s="36">
+        <f>+E17/E7</f>
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="36">
+        <f>+G17/G7</f>
+        <v>0.17100078802206461</v>
       </c>
       <c r="H26" s="36">
         <f>+H17/H7</f>
         <v>0.19479553903345725</v>
       </c>
+      <c r="I26" s="36">
+        <f>+I17/I7</f>
+        <v>0.23620933521923621</v>
+      </c>
+      <c r="J26" s="36">
+        <f>+J17/J7</f>
+        <v>0.21443158611300203</v>
+      </c>
+      <c r="K26" s="36">
+        <f>+K17/K7</f>
+        <v>0.21100917431192662</v>
+      </c>
       <c r="L26" s="36">
         <f>+L17/L7</f>
         <v>0.22790697674418606</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U26" s="36">
+        <f>+U17/U7</f>
+        <v>0.1409028727770178</v>
+      </c>
+      <c r="V26" s="36">
+        <f>+V17/V7</f>
+        <v>0.19760239760239759</v>
+      </c>
+      <c r="W26" s="36">
+        <f>+W17/W7</f>
+        <v>0.20520283791158814</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="36" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="E27" s="36">
+        <f>+E21/E7</f>
+        <v>0.15468750000000001</v>
+      </c>
+      <c r="G27" s="36">
+        <f>+G21/G7</f>
+        <v>0.12687155240346729</v>
       </c>
       <c r="H27" s="36">
         <f>+H21/H7</f>
         <v>0.16505576208178438</v>
       </c>
+      <c r="I27" s="36">
+        <f>+I21/I7</f>
+        <v>0.17043847241867044</v>
+      </c>
+      <c r="J27" s="36">
+        <f>+J21/J7</f>
+        <v>0.19196732471068753</v>
+      </c>
+      <c r="K27" s="36">
+        <f>+K21/K7</f>
+        <v>0.17784050811573748</v>
+      </c>
       <c r="L27" s="36">
         <f>+L21/L7</f>
         <v>0.18737541528239202</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U27" s="36">
+        <f>+U21/U7</f>
+        <v>0.11331509347925217</v>
+      </c>
+      <c r="V27" s="36">
+        <f>+V21/V7</f>
+        <v>0.16443556443556442</v>
+      </c>
+      <c r="W27" s="36">
+        <f>+W21/W7</f>
+        <v>0.16481717300345644</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="E28" s="36">
+        <f>+E20/E19</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="G28" s="36">
+        <f>+G20/G19</f>
+        <v>0.27149321266968324</v>
       </c>
       <c r="H28" s="36">
         <f>+H20/H19</f>
         <v>0.13953488372093023</v>
       </c>
+      <c r="I28" s="36">
+        <f>+I20/I19</f>
+        <v>0.24687500000000001</v>
+      </c>
+      <c r="J28" s="36">
+        <f>+J20/J19</f>
+        <v>0.16320474777448071</v>
+      </c>
+      <c r="K28" s="36">
+        <f>+K20/K19</f>
+        <v>0.18446601941747573</v>
+      </c>
       <c r="L28" s="36">
         <f>+L20/L19</f>
         <v>0.19886363636363635</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U28" s="36">
+        <f>+U20/U19</f>
+        <v>0.12035398230088495</v>
+      </c>
+      <c r="V28" s="36">
+        <f>+V20/V19</f>
+        <v>0.13002114164904863</v>
+      </c>
+      <c r="W28" s="36">
+        <f>+W20/W19</f>
+        <v>0.20246478873239437</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="I30" s="35">
+        <f>+I7/E7-1</f>
+        <v>0.10468750000000004</v>
+      </c>
+      <c r="K30" s="35">
+        <f>+K7/G7-1</f>
+        <v>0.11662726556343572</v>
       </c>
       <c r="L30" s="35">
         <f>+L7/H7-1</f>
         <v>0.11895910780669139</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>64</v>
+      <c r="V30" s="35">
+        <f>+V7/U7-1</f>
+        <v>0.14113087095303234</v>
+      </c>
+      <c r="W30" s="35">
+        <f>+W7/V7-1</f>
+        <v>9.8301698301698215E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="36">
+        <f>+H7/G7-1</f>
+        <v>5.9889676910953593E-2</v>
+      </c>
+      <c r="I31" s="36">
+        <f>+I7/H7-1</f>
+        <v>5.1301115241635609E-2</v>
+      </c>
+      <c r="J31" s="36">
+        <f>+J7/I7-1</f>
+        <v>3.8896746817538963E-2</v>
+      </c>
+      <c r="K31" s="36">
+        <f>+K7/J7-1</f>
+        <v>-3.539823008849563E-2</v>
+      </c>
+      <c r="L31" s="36">
+        <f>+L7/K7-1</f>
+        <v>6.2103034580098804E-2</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="33" t="s">
         <v>6</v>
       </c>
+      <c r="K38" s="33">
+        <v>1681</v>
+      </c>
       <c r="L38" s="33">
         <v>1513</v>
       </c>
     </row>
     <row r="39" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="33" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="K39" s="33">
+        <v>308</v>
       </c>
       <c r="L39" s="33">
         <v>365</v>
@@ -2007,7 +2944,10 @@
     </row>
     <row r="40" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="K40" s="32">
+        <v>353</v>
       </c>
       <c r="L40" s="32">
         <v>402</v>
@@ -2015,7 +2955,10 @@
     </row>
     <row r="41" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="K41" s="32">
+        <v>468</v>
       </c>
       <c r="L41" s="32">
         <v>478</v>
@@ -2023,7 +2966,43 @@
     </row>
     <row r="42" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="C42" s="32">
+        <f t="shared" ref="C42:K42" si="18">+SUM(C38:C41)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="32">
+        <f t="shared" si="18"/>
+        <v>2810</v>
       </c>
       <c r="L42" s="32">
         <f>+SUM(L38:L41)</f>
@@ -2032,7 +3011,10 @@
     </row>
     <row r="43" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="33" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="K43" s="33">
+        <v>238</v>
       </c>
       <c r="L43" s="33">
         <v>231</v>
@@ -2040,7 +3022,10 @@
     </row>
     <row r="44" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="32" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="K44" s="32">
+        <v>117</v>
       </c>
       <c r="L44" s="32">
         <v>116</v>
@@ -2048,7 +3033,10 @@
     </row>
     <row r="45" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="K45" s="32">
+        <v>214</v>
       </c>
       <c r="L45" s="32">
         <v>205</v>
@@ -2056,7 +3044,11 @@
     </row>
     <row r="46" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="K46" s="32">
+        <f>572+4133</f>
+        <v>4705</v>
       </c>
       <c r="L46" s="32">
         <f>609+4253</f>
@@ -2065,7 +3057,10 @@
     </row>
     <row r="47" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="K47" s="32">
+        <v>1126</v>
       </c>
       <c r="L47" s="32">
         <v>1129</v>
@@ -2073,7 +3068,10 @@
     </row>
     <row r="48" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="K48" s="32">
+        <v>620</v>
       </c>
       <c r="L48" s="32">
         <v>659</v>
@@ -2081,7 +3079,43 @@
     </row>
     <row r="49" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C49" s="32">
+        <f t="shared" ref="C49:K49" si="19">+SUM(C42:C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K49" s="32">
+        <f t="shared" si="19"/>
+        <v>9830</v>
       </c>
       <c r="L49" s="32">
         <f>+SUM(L42:L48)</f>
@@ -2091,7 +3125,10 @@
     <row r="50" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="K51" s="32">
+        <v>163</v>
       </c>
       <c r="L51" s="32">
         <v>174</v>
@@ -2099,7 +3136,10 @@
     </row>
     <row r="52" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="K52" s="32">
+        <v>326</v>
       </c>
       <c r="L52" s="32">
         <v>361</v>
@@ -2107,7 +3147,10 @@
     </row>
     <row r="53" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="K53" s="32">
+        <v>59</v>
       </c>
       <c r="L53" s="32">
         <v>48</v>
@@ -2115,7 +3158,10 @@
     </row>
     <row r="54" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="32" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="K54" s="32">
+        <v>3362</v>
       </c>
       <c r="L54" s="32">
         <v>3228</v>
@@ -2123,7 +3169,10 @@
     </row>
     <row r="55" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="32" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="K55" s="32">
+        <v>66</v>
       </c>
       <c r="L55" s="32">
         <v>67</v>
@@ -2131,7 +3180,10 @@
     </row>
     <row r="56" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="K56" s="33">
+        <v>0</v>
       </c>
       <c r="L56" s="33">
         <v>300</v>
@@ -2139,7 +3191,10 @@
     </row>
     <row r="57" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="32" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="K57" s="32">
+        <v>121</v>
       </c>
       <c r="L57" s="32">
         <v>159</v>
@@ -2147,7 +3202,43 @@
     </row>
     <row r="58" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="32" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="C58" s="32">
+        <f t="shared" ref="C58:K58" si="20">+SUM(C51:C57)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="32">
+        <f t="shared" si="20"/>
+        <v>4097</v>
       </c>
       <c r="L58" s="32">
         <f>+SUM(L51:L57)</f>
@@ -2156,7 +3247,10 @@
     </row>
     <row r="59" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="32" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="K59" s="32">
+        <v>600</v>
       </c>
       <c r="L59" s="32">
         <v>464</v>
@@ -2164,7 +3258,10 @@
     </row>
     <row r="60" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="K60" s="32">
+        <v>263</v>
       </c>
       <c r="L60" s="32">
         <v>250</v>
@@ -2172,7 +3269,10 @@
     </row>
     <row r="61" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="32" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="K61" s="32">
+        <v>178</v>
       </c>
       <c r="L61" s="32">
         <v>183</v>
@@ -2180,7 +3280,10 @@
     </row>
     <row r="62" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="32" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+      <c r="K62" s="32">
+        <v>42</v>
       </c>
       <c r="L62" s="32">
         <v>36</v>
@@ -2188,7 +3291,10 @@
     </row>
     <row r="63" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="33" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="K63" s="33">
+        <v>2285</v>
       </c>
       <c r="L63" s="33">
         <v>1986</v>
@@ -2196,91 +3302,295 @@
     </row>
     <row r="64" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+      <c r="K64" s="32">
+        <v>204</v>
       </c>
       <c r="L64" s="32">
         <v>230</v>
       </c>
     </row>
-    <row r="65" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="32" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="C65" s="32">
+        <f t="shared" ref="C65:K65" si="21">+SUM(C58:C64)</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="E65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J65" s="32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K65" s="32">
+        <f t="shared" si="21"/>
+        <v>7669</v>
       </c>
       <c r="L65" s="32">
         <f>+SUM(L58:L64)</f>
         <v>7486</v>
       </c>
     </row>
-    <row r="66" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="32" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="K67" s="32">
+        <v>2161</v>
       </c>
       <c r="L67" s="32">
         <v>2474</v>
       </c>
     </row>
-    <row r="68" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="32" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="K68" s="32">
+        <f>+K67+K65</f>
+        <v>9830</v>
       </c>
       <c r="L68" s="32">
         <f>+L67+L65</f>
         <v>9960</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="K70" s="32">
+        <f t="shared" ref="K70:L70" si="22">+K49-K65</f>
+        <v>2161</v>
       </c>
       <c r="L70" s="32">
         <f>+L49-L65</f>
         <v>2474</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="K71" s="2">
+        <f t="shared" ref="K71" si="23">+K70/K23</f>
+        <v>10.051162790697674</v>
       </c>
       <c r="L71" s="2">
         <f>+L70/L23</f>
         <v>11.453703703703704</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="K73" s="32">
+        <f t="shared" ref="K73:L73" si="24">+K38+K39+K43</f>
+        <v>2227</v>
       </c>
       <c r="L73" s="32">
         <f>+L38+L39+L43</f>
         <v>2109</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="K74" s="32">
+        <f t="shared" ref="K74:L74" si="25">+K56+K63</f>
+        <v>2285</v>
       </c>
       <c r="L74" s="32">
         <f>+L56+L63</f>
         <v>2286</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="K75" s="32">
+        <f t="shared" ref="K75" si="26">+K73-K74</f>
+        <v>-58</v>
       </c>
       <c r="L75" s="32">
         <f>+L73-L74</f>
         <v>-177</v>
       </c>
     </row>
+    <row r="79" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B79" s="38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G80" s="32">
+        <v>723</v>
+      </c>
+      <c r="H80" s="32">
+        <f>858-G80</f>
+        <v>135</v>
+      </c>
+      <c r="K80" s="32">
+        <v>494</v>
+      </c>
+      <c r="L80" s="32">
+        <f>706-K80</f>
+        <v>212</v>
+      </c>
+      <c r="U80" s="32">
+        <v>1531</v>
+      </c>
+      <c r="V80" s="32">
+        <v>2071</v>
+      </c>
+      <c r="W80" s="32">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="81" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G81" s="2">
+        <v>9</v>
+      </c>
+      <c r="H81" s="2">
+        <f>16-G81</f>
+        <v>7</v>
+      </c>
+      <c r="K81" s="2">
+        <v>7</v>
+      </c>
+      <c r="L81" s="2">
+        <f>16-K81</f>
+        <v>9</v>
+      </c>
+      <c r="U81" s="2">
+        <v>56</v>
+      </c>
+      <c r="V81" s="2">
+        <v>40</v>
+      </c>
+      <c r="W81" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B82" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G82" s="2">
+        <f>+G80-G81</f>
+        <v>714</v>
+      </c>
+      <c r="H82" s="2">
+        <f>+H80-H81</f>
+        <v>128</v>
+      </c>
+      <c r="K82" s="2">
+        <f>+K80-K81</f>
+        <v>487</v>
+      </c>
+      <c r="L82" s="2">
+        <f>+L80-L81</f>
+        <v>203</v>
+      </c>
+      <c r="U82" s="32">
+        <f>+U80-U81</f>
+        <v>1475</v>
+      </c>
+      <c r="V82" s="32">
+        <f>+V80-V81</f>
+        <v>2031</v>
+      </c>
+      <c r="W82" s="32">
+        <f>+W80-W81</f>
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="84" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B84" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="U84" s="32">
+        <f>+U82</f>
+        <v>1475</v>
+      </c>
+      <c r="V84" s="32">
+        <f>+V82</f>
+        <v>2031</v>
+      </c>
+      <c r="W84" s="32">
+        <f>+W82</f>
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="85" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B85" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="U85" s="2">
+        <f>+U84/U23</f>
+        <v>6.7045454545454541</v>
+      </c>
+      <c r="V85" s="2">
+        <f>+V84/V23</f>
+        <v>9.4027777777777786</v>
+      </c>
+      <c r="W85" s="2">
+        <f>+W84/W23</f>
+        <v>5.990654205607477</v>
+      </c>
+    </row>
+    <row r="86" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B86" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L1" r:id="rId1" xr:uid="{D5DBBD89-A61D-4F3A-9E1C-30B1DDD67C3E}"/>
+    <hyperlink ref="L1" r:id="rId1" display="Q224" xr:uid="{D5DBBD89-A61D-4F3A-9E1C-30B1DDD67C3E}"/>
+    <hyperlink ref="K1" r:id="rId2" display="Q124" xr:uid="{DF56E1CD-4488-4757-9A65-31755E2954D0}"/>
+    <hyperlink ref="I1" r:id="rId3" display="Q323" xr:uid="{5671B706-976C-4D5C-9ADF-C9F83D4468BA}"/>
+    <hyperlink ref="J1" r:id="rId4" xr:uid="{B00088EC-D5BD-487F-B3F1-EC27F64EE756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="L7" formulaRange="1"/>
+    <ignoredError sqref="K7:L7 I7" formulaRange="1"/>
+    <ignoredError sqref="J7:J22" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$WDAY new model, other updates
</commit_message>
<xml_diff>
--- a/$ADSK.xlsx
+++ b/$ADSK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619F2EC9-26FD-4A4B-B458-F7BCAD18A490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABD81A-CE8F-4C23-974C-CCA06265651B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="133">
   <si>
     <t>$ADSK</t>
   </si>
@@ -447,18 +447,6 @@
   </si>
   <si>
     <t>Q325</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>-</t>
@@ -737,39 +725,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -784,13 +739,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1174,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BFD011-71B1-4504-B133-A0FB7BFF1926}">
   <dimension ref="A2:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
@@ -1196,22 +1184,22 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="G5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="G5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="41"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1392,16 +1380,16 @@
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="G15" s="46">
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="G15" s="35">
         <v>45444</v>
       </c>
-      <c r="H15" s="48" t="s">
-        <v>134</v>
+      <c r="H15" s="37" t="s">
+        <v>130</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1418,10 +1406,10 @@
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="35"/>
+      <c r="D16" s="43"/>
       <c r="G16" s="12"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1439,10 +1427,10 @@
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D17" s="35"/>
+      <c r="D17" s="43"/>
       <c r="G17" s="12"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1457,10 +1445,10 @@
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="43"/>
       <c r="G18" s="12"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1475,8 +1463,8 @@
       <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
       <c r="G19" s="12"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -1510,11 +1498,11 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
       <c r="G22" s="12"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -1529,10 +1517,10 @@
       <c r="B23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="42">
         <v>1982</v>
       </c>
-      <c r="D23" s="35"/>
+      <c r="D23" s="43"/>
       <c r="G23" s="12"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1547,10 +1535,10 @@
       <c r="B24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="35"/>
+      <c r="D24" s="43"/>
       <c r="G24" s="12"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -1565,10 +1553,10 @@
       <c r="B25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="42">
         <v>1985</v>
       </c>
-      <c r="D25" s="35"/>
+      <c r="D25" s="43"/>
       <c r="G25" s="12"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -1581,8 +1569,8 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="35"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
       <c r="G26" s="12"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -1597,10 +1585,10 @@
       <c r="B27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="49">
+      <c r="C27" s="46">
         <v>14100</v>
       </c>
-      <c r="D27" s="50"/>
+      <c r="D27" s="47"/>
       <c r="G27" s="12"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -1613,8 +1601,8 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43"/>
       <c r="G28" s="12"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -1649,10 +1637,10 @@
       <c r="B30" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="37"/>
+      <c r="D30" s="49"/>
       <c r="G30" s="12"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
@@ -1686,11 +1674,11 @@
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="41"/>
       <c r="G33" s="12"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -1705,11 +1693,11 @@
       <c r="B34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="50">
         <f>+C6/'Financial Model'!P71</f>
         <v>28.049442198868228</v>
       </c>
-      <c r="D34" s="33"/>
+      <c r="D34" s="51"/>
       <c r="G34" s="12"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1724,11 +1712,11 @@
       <c r="B35" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="50">
         <f>+C8/SUM('Financial Model'!M7:P7)</f>
         <v>11.954232558139534</v>
       </c>
-      <c r="D35" s="33"/>
+      <c r="D35" s="51"/>
       <c r="G35" s="12"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
@@ -1743,11 +1731,11 @@
       <c r="B36" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="50">
         <f>+C6/SUM('Financial Model'!M22:P22)</f>
         <v>65.277899355462978</v>
       </c>
-      <c r="D36" s="33"/>
+      <c r="D36" s="51"/>
       <c r="G36" s="12"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
@@ -1762,11 +1750,11 @@
       <c r="B37" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="50">
         <f>+C6/'Financial Model'!P88</f>
         <v>61.41090265486725</v>
       </c>
-      <c r="D37" s="33"/>
+      <c r="D37" s="51"/>
       <c r="G37" s="12"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -1781,10 +1769,10 @@
       <c r="B38" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="42">
         <v>76</v>
       </c>
-      <c r="D38" s="35"/>
+      <c r="D38" s="43"/>
       <c r="G38" s="12"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
@@ -1797,8 +1785,8 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="12"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="35"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="43"/>
       <c r="G39" s="12"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
@@ -1810,7 +1798,7 @@
       <c r="O39" s="9"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G40" s="47"/>
+      <c r="G40" s="36"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -1822,6 +1810,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="G5:O5"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
@@ -1833,17 +1832,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C30:D30" r:id="rId1" display="Link" xr:uid="{136B0ED8-5FD6-4628-BBD0-474E201794EB}"/>
@@ -1858,11 +1846,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962F6E9D-1442-4F5B-A570-7043CF769B1D}">
   <dimension ref="B1:AD89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1921,7 +1909,7 @@
         <v>128</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="U1" s="17" t="s">
         <v>103</v>
@@ -2002,7 +1990,7 @@
         <v>43861</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Y2" s="21">
         <v>44592</v>
@@ -2303,8 +2291,16 @@
         <f>+SUM(P4:P6)</f>
         <v>1505</v>
       </c>
+      <c r="Q7" s="24">
+        <f>+P7*(1+Q30)</f>
+        <v>1700.6499999999999</v>
+      </c>
+      <c r="R7" s="24">
+        <f>+Q7*(1+R30)</f>
+        <v>1870.7149999999999</v>
+      </c>
       <c r="U7" s="24">
-        <f t="shared" ref="U7:Y7" si="5">+SUM(U4:U6)</f>
+        <f t="shared" ref="U7:X7" si="5">+SUM(U4:U6)</f>
         <v>0</v>
       </c>
       <c r="V7" s="24">
@@ -2331,6 +2327,10 @@
         <f t="shared" si="6"/>
         <v>5497</v>
       </c>
+      <c r="AB7" s="24">
+        <f>+SUM(O7:R7)</f>
+        <v>6493.3649999999998</v>
+      </c>
     </row>
     <row r="8" spans="2:30" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
@@ -2597,7 +2597,7 @@
         <v>140</v>
       </c>
       <c r="U11" s="23">
-        <f t="shared" ref="U11:Y11" si="12">SUM(U8:U10)</f>
+        <f t="shared" ref="U11:X11" si="12">SUM(U8:U10)</f>
         <v>0</v>
       </c>
       <c r="V11" s="23">
@@ -2685,8 +2685,16 @@
         <f>+P7-P11</f>
         <v>1365</v>
       </c>
+      <c r="Q12" s="24">
+        <f>+Q7-Q11</f>
+        <v>1700.6499999999999</v>
+      </c>
+      <c r="R12" s="24">
+        <f>+R7-R11</f>
+        <v>1870.7149999999999</v>
+      </c>
       <c r="U12" s="24">
-        <f t="shared" ref="U12:Y12" si="19">+U7-U11</f>
+        <f t="shared" ref="U12:X12" si="19">+U7-U11</f>
         <v>0</v>
       </c>
       <c r="V12" s="24">
@@ -2988,7 +2996,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
@@ -3048,8 +3056,16 @@
         <f>+P12-SUM(P13:P16)</f>
         <v>343</v>
       </c>
+      <c r="Q17" s="24">
+        <f>+Q12-SUM(Q13:Q16)</f>
+        <v>1700.6499999999999</v>
+      </c>
+      <c r="R17" s="24">
+        <f>+R12-SUM(R13:R16)</f>
+        <v>1870.7149999999999</v>
+      </c>
       <c r="U17" s="24">
-        <f t="shared" ref="U17:Y17" si="26">+U12-SUM(U13:U16)</f>
+        <f t="shared" ref="U17:X17" si="26">+U12-SUM(U13:U16)</f>
         <v>0</v>
       </c>
       <c r="V17" s="24">
@@ -3077,7 +3093,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
@@ -3126,6 +3142,14 @@
       <c r="P18" s="2">
         <v>9</v>
       </c>
+      <c r="Q18" s="2">
+        <f>+AVERAGE(L18:P18)</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R18" s="2">
+        <f>+AVERAGE(M18:Q18)</f>
+        <v>6.32</v>
+      </c>
       <c r="V18" s="23">
         <v>-17.7</v>
       </c>
@@ -3145,7 +3169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
@@ -3206,7 +3230,7 @@
         <v>352</v>
       </c>
       <c r="U19" s="23">
-        <f t="shared" ref="U19:Y19" si="33">+U17+U18</f>
+        <f t="shared" ref="U19:X19" si="33">+U17+U18</f>
         <v>0</v>
       </c>
       <c r="V19" s="23">
@@ -3234,7 +3258,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -3302,7 +3326,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="2:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
@@ -3315,7 +3339,7 @@
         <v>115</v>
       </c>
       <c r="E21" s="24">
-        <f t="shared" ref="E21:G21" si="37">+E19-E20</f>
+        <f t="shared" ref="E21:F21" si="37">+E19-E20</f>
         <v>137</v>
       </c>
       <c r="F21" s="24">
@@ -3363,7 +3387,7 @@
         <v>282</v>
       </c>
       <c r="U21" s="24">
-        <f t="shared" ref="U21:Y21" si="40">+U19-U20</f>
+        <f t="shared" ref="U21:X21" si="40">+U19-U20</f>
         <v>0</v>
       </c>
       <c r="V21" s="24">
@@ -3391,92 +3415,92 @@
         <v>906</v>
       </c>
     </row>
-    <row r="22" spans="2:27" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:28" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="25">
-        <f>+C21/C23</f>
+        <f t="shared" ref="C22:J22" si="42">+C21/C23</f>
         <v>0.70270270270270274</v>
       </c>
       <c r="D22" s="25">
-        <f>+D21/D23</f>
+        <f t="shared" si="42"/>
         <v>0.52272727272727271</v>
       </c>
       <c r="E22" s="25">
-        <f>+E21/E23</f>
+        <f t="shared" si="42"/>
         <v>0.62272727272727268</v>
       </c>
       <c r="F22" s="25">
-        <f>+F21/F23</f>
+        <f t="shared" si="42"/>
         <v>0.40454545454545454</v>
       </c>
       <c r="G22" s="25">
-        <f>+G21/G23</f>
+        <f t="shared" si="42"/>
         <v>0.67281105990783407</v>
       </c>
       <c r="H22" s="25">
-        <f>+H21/H23</f>
+        <f t="shared" si="42"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="I22" s="25">
-        <f>+I21/I23</f>
+        <f t="shared" si="42"/>
         <v>0.9124423963133641</v>
       </c>
       <c r="J22" s="25">
-        <f>+J21/J23</f>
+        <f t="shared" si="42"/>
         <v>1.3564814814814814</v>
       </c>
       <c r="K22" s="25">
-        <f t="shared" ref="K22:P22" si="42">+K21/K23</f>
+        <f t="shared" ref="K22:P22" si="43">+K21/K23</f>
         <v>0.74883720930232556</v>
       </c>
       <c r="L22" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.0373831775700935</v>
       </c>
       <c r="M22" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.1261682242990654</v>
       </c>
       <c r="N22" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.3177570093457944</v>
       </c>
       <c r="O22" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.172093023255814</v>
       </c>
       <c r="P22" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1.3055555555555556</v>
       </c>
       <c r="V22" s="25">
-        <f>+V21/V23</f>
+        <f t="shared" ref="V22:AA22" si="44">+V21/V23</f>
         <v>-0.36911831886706264</v>
       </c>
       <c r="W22" s="25">
-        <f>+W21/W23</f>
+        <f t="shared" si="44"/>
         <v>0.97633136094674566</v>
       </c>
       <c r="X22" s="25">
-        <f>+X21/X23</f>
+        <f t="shared" si="44"/>
         <v>5.5068368277119406</v>
       </c>
       <c r="Y22" s="25">
-        <f>+Y21/Y23</f>
+        <f t="shared" si="44"/>
         <v>2.2590909090909093</v>
       </c>
       <c r="Z22" s="25">
-        <f>+Z21/Z23</f>
+        <f t="shared" si="44"/>
         <v>3.8101851851851851</v>
       </c>
       <c r="AA22" s="25">
-        <f>+AA21/AA23</f>
+        <f t="shared" si="44"/>
         <v>4.2336448598130838</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
@@ -3544,401 +3568,410 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="2:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="27">
-        <f>+C12/C7</f>
+        <f t="shared" ref="C25:J25" si="45">+C12/C7</f>
         <v>0.90697674418604646</v>
       </c>
       <c r="D25" s="27">
-        <f>+D12/D7</f>
+        <f t="shared" si="45"/>
         <v>0.9</v>
       </c>
       <c r="E25" s="27">
-        <f>+E12/E7</f>
+        <f t="shared" si="45"/>
         <v>0.9040852575488455</v>
       </c>
       <c r="F25" s="27">
-        <f>+F12/F7</f>
+        <f t="shared" si="45"/>
         <v>0.90751445086705207</v>
       </c>
       <c r="G25" s="27">
-        <f>+G12/G7</f>
+        <f t="shared" si="45"/>
         <v>0.9</v>
       </c>
       <c r="H25" s="27">
-        <f>+H12/H7</f>
+        <f t="shared" si="45"/>
         <v>0.90379951495553756</v>
       </c>
       <c r="I25" s="27">
-        <f>+I12/I7</f>
+        <f t="shared" si="45"/>
         <v>0.90625</v>
       </c>
       <c r="J25" s="27">
-        <f>+J12/J7</f>
+        <f t="shared" si="45"/>
         <v>0.90591805766312594</v>
       </c>
       <c r="K25" s="27">
-        <f t="shared" ref="K25:P25" si="43">+K12/K7</f>
+        <f t="shared" ref="K25:P25" si="46">+K12/K7</f>
         <v>0.89992119779353819</v>
       </c>
       <c r="L25" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.90557620817843865</v>
       </c>
       <c r="M25" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.91018387553041014</v>
       </c>
       <c r="N25" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.91150442477876104</v>
       </c>
       <c r="O25" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.90331686661961896</v>
       </c>
       <c r="P25" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>0.90697674418604646</v>
       </c>
       <c r="V25" s="27">
-        <f>+V12/V7</f>
+        <f t="shared" ref="V25:AA25" si="47">+V12/V7</f>
         <v>0.88874620593042253</v>
       </c>
       <c r="W25" s="27">
-        <f>+W12/W7</f>
+        <f t="shared" si="47"/>
         <v>0.90077268423785239</v>
       </c>
       <c r="X25" s="27">
-        <f>+X12/X7</f>
+        <f t="shared" si="47"/>
         <v>0.9110647952722668</v>
       </c>
       <c r="Y25" s="27">
-        <f>+Y12/Y7</f>
+        <f t="shared" si="47"/>
         <v>0.90469676242590058</v>
       </c>
       <c r="Z25" s="27">
-        <f>+Z12/Z7</f>
+        <f t="shared" si="47"/>
         <v>0.90409590409590412</v>
       </c>
       <c r="AA25" s="27">
-        <f>+AA12/AA7</f>
+        <f t="shared" si="47"/>
         <v>0.90704020374749861</v>
       </c>
-    </row>
-    <row r="26" spans="2:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB25" s="27">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="27" t="s">
         <v>56</v>
       </c>
       <c r="C26" s="27">
-        <f>+C17/C7</f>
+        <f t="shared" ref="C26:J26" si="48">+C17/C7</f>
         <v>0.13549039433771487</v>
       </c>
       <c r="D26" s="27">
-        <f>+D17/D7</f>
+        <f t="shared" si="48"/>
         <v>0.13962264150943396</v>
       </c>
       <c r="E26" s="27">
-        <f>+E17/E7</f>
+        <f t="shared" si="48"/>
         <v>0.17140319715808169</v>
       </c>
       <c r="F26" s="27">
-        <f>+F17/F7</f>
+        <f t="shared" si="48"/>
         <v>0.1180842279108175</v>
       </c>
       <c r="G26" s="27">
-        <f>+G17/G7</f>
+        <f t="shared" si="48"/>
         <v>0.18290598290598289</v>
       </c>
       <c r="H26" s="27">
-        <f>+H17/H7</f>
+        <f t="shared" si="48"/>
         <v>0.19563459983831852</v>
       </c>
       <c r="I26" s="27">
-        <f>+I17/I7</f>
+        <f t="shared" si="48"/>
         <v>0.2</v>
       </c>
       <c r="J26" s="27">
-        <f>+J17/J7</f>
+        <f t="shared" si="48"/>
         <v>0.2101669195751138</v>
       </c>
       <c r="K26" s="27">
-        <f t="shared" ref="K26:P26" si="44">+K17/K7</f>
+        <f t="shared" ref="K26:P26" si="49">+K17/K7</f>
         <v>0.17100078802206461</v>
       </c>
       <c r="L26" s="27">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>0.19479553903345725</v>
       </c>
       <c r="M26" s="27">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>0.23620933521923621</v>
       </c>
       <c r="N26" s="27">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>0.21443158611300203</v>
       </c>
       <c r="O26" s="27">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>0.21100917431192662</v>
       </c>
       <c r="P26" s="27">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>0.22790697674418606</v>
       </c>
       <c r="V26" s="27">
-        <f>+V17/V7</f>
+        <f t="shared" ref="V26:AA26" si="50">+V17/V7</f>
         <v>-9.7283835317923568E-3</v>
       </c>
       <c r="W26" s="27">
-        <f>+W17/W7</f>
+        <f t="shared" si="50"/>
         <v>0.10475521485508352</v>
       </c>
       <c r="X26" s="27">
-        <f>+X17/X7</f>
+        <f t="shared" si="50"/>
         <v>0.16597192908400166</v>
       </c>
       <c r="Y26" s="27">
-        <f>+Y17/Y7</f>
+        <f t="shared" si="50"/>
         <v>0.1409028727770178</v>
       </c>
       <c r="Z26" s="27">
-        <f>+Z17/Z7</f>
+        <f t="shared" si="50"/>
         <v>0.19760239760239759</v>
       </c>
       <c r="AA26" s="27">
-        <f>+AA17/AA7</f>
+        <f t="shared" si="50"/>
         <v>0.20520283791158814</v>
       </c>
     </row>
-    <row r="27" spans="2:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="27" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="27">
-        <f>+C21/C7</f>
+        <f t="shared" ref="C27:J27" si="51">+C21/C7</f>
         <v>0.15773508594539939</v>
       </c>
       <c r="D27" s="27">
-        <f>+D21/D7</f>
+        <f t="shared" si="51"/>
         <v>0.10849056603773585</v>
       </c>
       <c r="E27" s="27">
-        <f>+E21/E7</f>
+        <f t="shared" si="51"/>
         <v>0.1216696269982238</v>
       </c>
       <c r="F27" s="27">
-        <f>+F21/F7</f>
+        <f t="shared" si="51"/>
         <v>7.3492981007431873E-2</v>
       </c>
       <c r="G27" s="27">
-        <f>+G21/G7</f>
+        <f t="shared" si="51"/>
         <v>0.12478632478632479</v>
       </c>
       <c r="H27" s="27">
-        <f>+H21/H7</f>
+        <f t="shared" si="51"/>
         <v>0.15036378334680678</v>
       </c>
       <c r="I27" s="27">
-        <f>+I21/I7</f>
+        <f t="shared" si="51"/>
         <v>0.15468750000000001</v>
       </c>
       <c r="J27" s="27">
-        <f>+J21/J7</f>
+        <f t="shared" si="51"/>
         <v>0.22230652503793627</v>
       </c>
       <c r="K27" s="27">
-        <f t="shared" ref="K27:P27" si="45">+K21/K7</f>
+        <f t="shared" ref="K27:P27" si="52">+K21/K7</f>
         <v>0.12687155240346729</v>
       </c>
       <c r="L27" s="27">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>0.16505576208178438</v>
       </c>
       <c r="M27" s="27">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>0.17043847241867044</v>
       </c>
       <c r="N27" s="27">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>0.19196732471068753</v>
       </c>
       <c r="O27" s="27">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>0.17784050811573748</v>
       </c>
       <c r="P27" s="27">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>0.18737541528239202</v>
       </c>
       <c r="V27" s="27">
-        <f>+V21/V7</f>
+        <f t="shared" ref="V27:AA27" si="53">+V21/V7</f>
         <v>-3.1442135574752901E-2</v>
       </c>
       <c r="W27" s="27">
-        <f>+W21/W7</f>
+        <f t="shared" si="53"/>
         <v>6.5510185383135328E-2</v>
       </c>
       <c r="X27" s="27">
-        <f>+X21/X7</f>
+        <f t="shared" si="53"/>
         <v>0.31875263824398475</v>
       </c>
       <c r="Y27" s="27">
-        <f>+Y21/Y7</f>
+        <f t="shared" si="53"/>
         <v>0.11331509347925217</v>
       </c>
       <c r="Z27" s="27">
-        <f>+Z21/Z7</f>
+        <f t="shared" si="53"/>
         <v>0.16443556443556442</v>
       </c>
       <c r="AA27" s="27">
-        <f>+AA21/AA7</f>
+        <f t="shared" si="53"/>
         <v>0.16481717300345644</v>
       </c>
     </row>
-    <row r="28" spans="2:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="27" t="s">
         <v>58</v>
       </c>
       <c r="C28" s="27">
-        <f>+C20/C19</f>
+        <f t="shared" ref="C28:J28" si="54">+C20/C19</f>
         <v>-0.19083969465648856</v>
       </c>
       <c r="D28" s="27">
-        <f>+D20/D19</f>
+        <f t="shared" si="54"/>
         <v>0.17266187050359713</v>
       </c>
       <c r="E28" s="27">
-        <f>+E20/E19</f>
+        <f t="shared" si="54"/>
         <v>0.27127659574468083</v>
       </c>
       <c r="F28" s="27">
-        <f>+F20/F19</f>
+        <f t="shared" si="54"/>
         <v>0.16822429906542055</v>
       </c>
       <c r="G28" s="27">
-        <f>+G20/G19</f>
+        <f t="shared" si="54"/>
         <v>0.25128205128205128</v>
       </c>
       <c r="H28" s="27">
-        <f>+H20/H19</f>
+        <f t="shared" si="54"/>
         <v>0.19827586206896552</v>
       </c>
       <c r="I28" s="27">
-        <f>+I20/I19</f>
+        <f t="shared" si="54"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="J28" s="27">
-        <f>+J20/J19</f>
+        <f t="shared" si="54"/>
         <v>-5.7761732851985562E-2</v>
       </c>
       <c r="K28" s="27">
-        <f t="shared" ref="K28:P28" si="46">+K20/K19</f>
+        <f t="shared" ref="K28:P28" si="55">+K20/K19</f>
         <v>0.27149321266968324</v>
       </c>
       <c r="L28" s="27">
-        <f t="shared" si="46"/>
+        <f t="shared" si="55"/>
         <v>0.13953488372093023</v>
       </c>
       <c r="M28" s="27">
-        <f t="shared" si="46"/>
+        <f t="shared" si="55"/>
         <v>0.24687500000000001</v>
       </c>
       <c r="N28" s="27">
-        <f t="shared" si="46"/>
+        <f t="shared" si="55"/>
         <v>0.16320474777448071</v>
       </c>
       <c r="O28" s="27">
-        <f t="shared" si="46"/>
+        <f t="shared" si="55"/>
         <v>0.18446601941747573</v>
       </c>
       <c r="P28" s="27">
-        <f t="shared" si="46"/>
+        <f t="shared" si="55"/>
         <v>0.19886363636363635</v>
       </c>
       <c r="V28" s="27">
-        <f>+V20/V19</f>
+        <f t="shared" ref="V28:AA28" si="56">+V20/V19</f>
         <v>-0.89227166276346603</v>
       </c>
       <c r="W28" s="27">
-        <f>+W20/W19</f>
+        <f t="shared" si="56"/>
         <v>0.27238805970149249</v>
       </c>
       <c r="X28" s="27">
-        <f>+X20/X19</f>
+        <f t="shared" si="56"/>
         <v>-1.2099871959026891</v>
       </c>
       <c r="Y28" s="27">
-        <f>+Y20/Y19</f>
+        <f t="shared" si="56"/>
         <v>0.12035398230088495</v>
       </c>
       <c r="Z28" s="27">
-        <f>+Z20/Z19</f>
+        <f t="shared" si="56"/>
         <v>0.13002114164904863</v>
       </c>
       <c r="AA28" s="27">
-        <f>+AA20/AA19</f>
+        <f t="shared" si="56"/>
         <v>0.20246478873239437</v>
       </c>
     </row>
-    <row r="30" spans="2:27" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:28" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>133</v>
+      <c r="C30" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>129</v>
       </c>
       <c r="G30" s="26">
-        <f>+G7/C7-1</f>
+        <f t="shared" ref="G30:P30" si="57">+G7/C7-1</f>
         <v>0.18301314459049545</v>
       </c>
       <c r="H30" s="26">
-        <f>+H7/D7-1</f>
+        <f t="shared" si="57"/>
         <v>0.16698113207547172</v>
       </c>
       <c r="I30" s="26">
-        <f>+I7/E7-1</f>
+        <f t="shared" si="57"/>
         <v>0.13676731793960917</v>
       </c>
       <c r="J30" s="26">
-        <f>+J7/F7-1</f>
+        <f t="shared" si="57"/>
         <v>8.8356729975227033E-2</v>
       </c>
       <c r="K30" s="26">
-        <f>+K7/G7-1</f>
+        <f t="shared" si="57"/>
         <v>8.4615384615384537E-2</v>
       </c>
       <c r="L30" s="26">
-        <f>+L7/H7-1</f>
+        <f t="shared" si="57"/>
         <v>8.730800323362975E-2</v>
       </c>
       <c r="M30" s="26">
-        <f>+M7/I7-1</f>
+        <f t="shared" si="57"/>
         <v>0.10468750000000004</v>
       </c>
       <c r="N30" s="26">
-        <f>+N7/J7-1</f>
+        <f t="shared" si="57"/>
         <v>0.11456752655538693</v>
       </c>
       <c r="O30" s="26">
-        <f>+O7/K7-1</f>
+        <f t="shared" si="57"/>
         <v>0.11662726556343572</v>
       </c>
       <c r="P30" s="26">
-        <f>+P7/L7-1</f>
+        <f t="shared" si="57"/>
         <v>0.11895910780669139</v>
+      </c>
+      <c r="Q30" s="26">
+        <v>0.13</v>
+      </c>
+      <c r="R30" s="26">
+        <v>0.1</v>
       </c>
       <c r="W30" s="26">
         <f>+W7/V7-1</f>
@@ -3960,86 +3993,101 @@
         <f>+AA7/Z7-1</f>
         <v>9.8301698301698215E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:27" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB30" s="26">
+        <f>+AB7/AA7-1</f>
+        <v>0.18125613971257049</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>133</v>
+      <c r="C31" s="34" t="s">
+        <v>129</v>
       </c>
       <c r="D31" s="27">
-        <f>+D7/C7-1</f>
+        <f t="shared" ref="D31:R31" si="58">+D7/C7-1</f>
         <v>7.1789686552072851E-2</v>
       </c>
       <c r="E31" s="27">
-        <f>+E7/D7-1</f>
+        <f t="shared" si="58"/>
         <v>6.2264150943396324E-2</v>
       </c>
       <c r="F31" s="27">
-        <f>+F7/E7-1</f>
+        <f t="shared" si="58"/>
         <v>7.5488454706927222E-2</v>
       </c>
       <c r="G31" s="27">
-        <f>+G7/F7-1</f>
+        <f t="shared" si="58"/>
         <v>-3.3856317093311272E-2</v>
       </c>
       <c r="H31" s="27">
-        <f>+H7/G7-1</f>
+        <f t="shared" si="58"/>
         <v>5.7264957264957284E-2</v>
       </c>
       <c r="I31" s="27">
-        <f>+I7/H7-1</f>
+        <f t="shared" si="58"/>
         <v>3.4761519805982299E-2</v>
       </c>
       <c r="J31" s="27">
-        <f>+J7/I7-1</f>
+        <f t="shared" si="58"/>
         <v>2.9687500000000089E-2</v>
       </c>
       <c r="K31" s="27">
-        <f>+K7/J7-1</f>
+        <f t="shared" si="58"/>
         <v>-3.7177541729893737E-2</v>
       </c>
       <c r="L31" s="27">
-        <f>+L7/K7-1</f>
+        <f t="shared" si="58"/>
         <v>5.9889676910953593E-2</v>
       </c>
       <c r="M31" s="27">
-        <f>+M7/L7-1</f>
+        <f t="shared" si="58"/>
         <v>5.1301115241635609E-2</v>
       </c>
       <c r="N31" s="27">
-        <f>+N7/M7-1</f>
+        <f t="shared" si="58"/>
         <v>3.8896746817538963E-2</v>
       </c>
       <c r="O31" s="27">
-        <f>+O7/N7-1</f>
+        <f t="shared" si="58"/>
         <v>-3.539823008849563E-2</v>
       </c>
       <c r="P31" s="27">
-        <f>+P7/O7-1</f>
+        <f t="shared" si="58"/>
         <v>6.2103034580098804E-2</v>
       </c>
-      <c r="U31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="V31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="W31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="X31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z31" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA31" s="45" t="s">
-        <v>133</v>
+      <c r="Q31" s="27">
+        <f t="shared" si="58"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="R31" s="27">
+        <f t="shared" si="58"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="U31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="V31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="W31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="X31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB31" s="34" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
@@ -4096,55 +4144,55 @@
         <v>65</v>
       </c>
       <c r="C42" s="23">
-        <f t="shared" ref="C42:G42" si="47">+SUM(C38:C41)</f>
+        <f t="shared" ref="C42:F42" si="59">+SUM(C38:C41)</f>
         <v>0</v>
       </c>
       <c r="D42" s="23">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="E42" s="23">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="F42" s="23">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="G42" s="23">
-        <f t="shared" ref="G42:O42" si="48">+SUM(G38:G41)</f>
+        <f t="shared" ref="G42:O42" si="60">+SUM(G38:G41)</f>
         <v>0</v>
       </c>
       <c r="H42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="I42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="J42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="K42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="L42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="N42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="O42" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>2810</v>
       </c>
       <c r="P42" s="23">
@@ -4225,55 +4273,55 @@
         <v>72</v>
       </c>
       <c r="C49" s="23">
-        <f t="shared" ref="C49:G49" si="49">+SUM(C42:C48)</f>
+        <f t="shared" ref="C49:F49" si="61">+SUM(C42:C48)</f>
         <v>0</v>
       </c>
       <c r="D49" s="23">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="E49" s="23">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F49" s="23">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="G49" s="23">
-        <f t="shared" ref="G49:O49" si="50">+SUM(G42:G48)</f>
+        <f t="shared" ref="G49:O49" si="62">+SUM(G42:G48)</f>
         <v>0</v>
       </c>
       <c r="H49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="I49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="J49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="K49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="L49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="M49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="N49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O49" s="23">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>9830</v>
       </c>
       <c r="P49" s="23">
@@ -4364,55 +4412,55 @@
         <v>79</v>
       </c>
       <c r="C58" s="23">
-        <f t="shared" ref="C58:G58" si="51">+SUM(C51:C57)</f>
+        <f t="shared" ref="C58:F58" si="63">+SUM(C51:C57)</f>
         <v>0</v>
       </c>
       <c r="D58" s="23">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="E58" s="23">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="F58" s="23">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G58" s="23">
-        <f t="shared" ref="G58:O58" si="52">+SUM(G51:G57)</f>
+        <f t="shared" ref="G58:O58" si="64">+SUM(G51:G57)</f>
         <v>0</v>
       </c>
       <c r="H58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="J58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="L58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="M58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="N58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="O58" s="23">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>4097</v>
       </c>
       <c r="P58" s="23">
@@ -4491,55 +4539,55 @@
         <v>86</v>
       </c>
       <c r="C65" s="23">
-        <f t="shared" ref="C65:G65" si="53">+SUM(C58:C64)</f>
+        <f t="shared" ref="C65:F65" si="65">+SUM(C58:C64)</f>
         <v>0</v>
       </c>
       <c r="D65" s="23">
-        <f t="shared" si="53"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="E65" s="23">
-        <f t="shared" si="53"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="F65" s="23">
-        <f t="shared" si="53"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G65" s="23">
-        <f t="shared" ref="G65:O65" si="54">+SUM(G58:G64)</f>
+        <f t="shared" ref="G65:O65" si="66">+SUM(G58:G64)</f>
         <v>0</v>
       </c>
       <c r="H65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="I65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="J65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="L65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="M65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="N65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="O65" s="23">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>7669</v>
       </c>
       <c r="P65" s="23">
@@ -4577,7 +4625,7 @@
         <v>90</v>
       </c>
       <c r="O70" s="23">
-        <f t="shared" ref="O70" si="55">+O49-O65</f>
+        <f t="shared" ref="O70" si="67">+O49-O65</f>
         <v>2161</v>
       </c>
       <c r="P70" s="23">
@@ -4590,7 +4638,7 @@
         <v>91</v>
       </c>
       <c r="O71" s="2">
-        <f t="shared" ref="O71" si="56">+O70/O23</f>
+        <f t="shared" ref="O71" si="68">+O70/O23</f>
         <v>10.051162790697674</v>
       </c>
       <c r="P71" s="2">
@@ -4603,7 +4651,7 @@
         <v>6</v>
       </c>
       <c r="O73" s="23">
-        <f t="shared" ref="O73" si="57">+O38+O39+O43</f>
+        <f t="shared" ref="O73" si="69">+O38+O39+O43</f>
         <v>2227</v>
       </c>
       <c r="P73" s="23">
@@ -4616,7 +4664,7 @@
         <v>7</v>
       </c>
       <c r="O74" s="23">
-        <f t="shared" ref="O74" si="58">+O56+O63</f>
+        <f t="shared" ref="O74" si="70">+O56+O63</f>
         <v>2285</v>
       </c>
       <c r="P74" s="23">
@@ -4629,7 +4677,7 @@
         <v>8</v>
       </c>
       <c r="O75" s="23">
-        <f t="shared" ref="O75" si="59">+O73-O74</f>
+        <f t="shared" ref="O75" si="71">+O73-O74</f>
         <v>-58</v>
       </c>
       <c r="P75" s="23">
@@ -4848,59 +4896,59 @@
         <v>95</v>
       </c>
       <c r="C85" s="23">
-        <f>+C83-C84</f>
+        <f t="shared" ref="C85:P85" si="72">+C83-C84</f>
         <v>316</v>
       </c>
       <c r="D85" s="23">
-        <f>+D83-D84</f>
+        <f t="shared" si="72"/>
         <v>186</v>
       </c>
       <c r="E85" s="23">
-        <f>+E83-E84</f>
+        <f t="shared" si="72"/>
         <v>275</v>
       </c>
       <c r="F85" s="23">
-        <f>+F83-F84</f>
+        <f t="shared" si="72"/>
         <v>698</v>
       </c>
       <c r="G85" s="23">
-        <f>+G83-G84</f>
+        <f t="shared" si="72"/>
         <v>422</v>
       </c>
       <c r="H85" s="23">
-        <f>+H83-H84</f>
+        <f t="shared" si="72"/>
         <v>246</v>
       </c>
       <c r="I85" s="23">
-        <f>+I83-I84</f>
+        <f t="shared" si="72"/>
         <v>460</v>
       </c>
       <c r="J85" s="23">
-        <f>+J83-J84</f>
+        <f t="shared" si="72"/>
         <v>903</v>
       </c>
       <c r="K85" s="2">
-        <f>+K83-K84</f>
+        <f t="shared" si="72"/>
         <v>714</v>
       </c>
       <c r="L85" s="2">
-        <f>+L83-L84</f>
+        <f t="shared" si="72"/>
         <v>128</v>
       </c>
       <c r="M85" s="2">
-        <f>+M83-M84</f>
+        <f t="shared" si="72"/>
         <v>13</v>
       </c>
       <c r="N85" s="2">
-        <f>+N83-N84</f>
+        <f t="shared" si="72"/>
         <v>427</v>
       </c>
       <c r="O85" s="2">
-        <f>+O83-O84</f>
+        <f t="shared" si="72"/>
         <v>487</v>
       </c>
       <c r="P85" s="2">
-        <f>+P83-P84</f>
+        <f t="shared" si="72"/>
         <v>203</v>
       </c>
       <c r="V85" s="23">
@@ -4908,11 +4956,11 @@
         <v>310.10000000000002</v>
       </c>
       <c r="W85" s="23">
-        <f t="shared" ref="W85:X85" si="60">+W83-W84</f>
+        <f t="shared" ref="W85:X85" si="73">+W83-W84</f>
         <v>1361.8999999999999</v>
       </c>
       <c r="X85" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="73"/>
         <v>1346.1000000000001</v>
       </c>
       <c r="Y85" s="23">
@@ -4945,84 +4993,84 @@
         <v>1130</v>
       </c>
       <c r="V87" s="23">
-        <f>+V85</f>
+        <f t="shared" ref="V87:AA87" si="74">+V85</f>
         <v>310.10000000000002</v>
       </c>
       <c r="W87" s="23">
-        <f>+W85</f>
+        <f t="shared" si="74"/>
         <v>1361.8999999999999</v>
       </c>
       <c r="X87" s="23">
-        <f>+X85</f>
+        <f t="shared" si="74"/>
         <v>1346.1000000000001</v>
       </c>
       <c r="Y87" s="23">
-        <f>+Y85</f>
+        <f t="shared" si="74"/>
         <v>1475</v>
       </c>
       <c r="Z87" s="23">
-        <f>+Z85</f>
+        <f t="shared" si="74"/>
         <v>2031</v>
       </c>
       <c r="AA87" s="23">
-        <f>+AA85</f>
+        <f t="shared" si="74"/>
         <v>1282</v>
       </c>
     </row>
-    <row r="88" spans="2:27" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="51" t="s">
+    <row r="88" spans="2:27" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="N88" s="51">
+      <c r="N88" s="38">
         <f>+N87/N23</f>
         <v>5.990654205607477</v>
       </c>
-      <c r="O88" s="51">
+      <c r="O88" s="38">
         <f>+O87/O23</f>
         <v>4.9069767441860463</v>
       </c>
-      <c r="P88" s="51">
+      <c r="P88" s="38">
         <f>+P87/P23</f>
         <v>5.2314814814814818</v>
       </c>
-      <c r="V88" s="51">
-        <f>+V87/V23</f>
+      <c r="V88" s="38">
+        <f t="shared" ref="V88:AA88" si="75">+V87/V23</f>
         <v>1.4166285975331203</v>
       </c>
-      <c r="W88" s="51">
-        <f>+W87/W23</f>
+      <c r="W88" s="38">
+        <f t="shared" si="75"/>
         <v>6.1989076012744651</v>
       </c>
-      <c r="X88" s="51">
-        <f>+X87/X23</f>
+      <c r="X88" s="38">
+        <f t="shared" si="75"/>
         <v>6.135369188696445</v>
       </c>
-      <c r="Y88" s="51">
-        <f>+Y87/Y23</f>
+      <c r="Y88" s="38">
+        <f t="shared" si="75"/>
         <v>6.7045454545454541</v>
       </c>
-      <c r="Z88" s="51">
-        <f>+Z87/Z23</f>
+      <c r="Z88" s="38">
+        <f t="shared" si="75"/>
         <v>9.4027777777777786</v>
       </c>
-      <c r="AA88" s="51">
-        <f>+AA87/AA23</f>
+      <c r="AA88" s="38">
+        <f t="shared" si="75"/>
         <v>5.990654205607477</v>
       </c>
     </row>
-    <row r="89" spans="2:27" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="43" t="s">
+    <row r="89" spans="2:27" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N89" s="43">
+      <c r="N89" s="32">
         <f>+N77/N88</f>
         <v>40.64330733229329</v>
       </c>
-      <c r="O89" s="43">
+      <c r="O89" s="32">
         <f>+O77/O88</f>
         <v>43.377014218009478</v>
       </c>
-      <c r="P89" s="43">
+      <c r="P89" s="32">
         <f>+P77/P88</f>
         <v>47.313557522123894</v>
       </c>

</xml_diff>

<commit_message>
$ADSK $WDAY Q325 results
</commit_message>
<xml_diff>
--- a/$ADSK.xlsx
+++ b/$ADSK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABD81A-CE8F-4C23-974C-CCA06265651B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5555A5E9-4566-4FF5-83CE-C13EA74046B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBC686BB-2718-4D0D-A16A-D84819AF3AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
   <si>
     <t>$ADSK</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>Q425</t>
+  </si>
+  <si>
+    <t>ESTC's ex CFO announced as new CFO starting in December</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -779,6 +782,7 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1162,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BFD011-71B1-4504-B133-A0FB7BFF1926}">
   <dimension ref="A2:U40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>321.27</v>
+        <v>287</v>
       </c>
       <c r="D6" s="30"/>
       <c r="G6" s="12"/>
@@ -1224,11 +1228,12 @@
         <v>4</v>
       </c>
       <c r="C7" s="4">
-        <v>216</v>
+        <f>+'Financial Model'!Q23</f>
+        <v>215</v>
       </c>
       <c r="D7" s="30" t="str">
         <f>+$C$29</f>
-        <v>Q225</v>
+        <v>Q325</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="8"/>
@@ -1250,11 +1255,15 @@
       </c>
       <c r="C8" s="14">
         <f>C6*C7</f>
-        <v>69394.319999999992</v>
+        <v>61705</v>
       </c>
       <c r="D8" s="30"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="35">
+        <v>45597</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -1271,12 +1280,12 @@
         <v>6</v>
       </c>
       <c r="C9" s="14">
-        <f>+'Financial Model'!P73</f>
-        <v>2109</v>
+        <f>+'Financial Model'!Q83</f>
+        <v>209</v>
       </c>
       <c r="D9" s="30" t="str">
         <f t="shared" ref="D9:D11" si="0">+$C$29</f>
-        <v>Q225</v>
+        <v>Q325</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="8"/>
@@ -1296,12 +1305,12 @@
         <v>7</v>
       </c>
       <c r="C10" s="14">
-        <f>+'Financial Model'!P74</f>
-        <v>2286</v>
+        <f>+'Financial Model'!Q84</f>
+        <v>10</v>
       </c>
       <c r="D10" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>Q225</v>
+        <v>Q325</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="8"/>
@@ -1322,11 +1331,11 @@
       </c>
       <c r="C11" s="14">
         <f>C9-C10</f>
-        <v>-177</v>
+        <v>199</v>
       </c>
       <c r="D11" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>Q225</v>
+        <v>Q325</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="8"/>
@@ -1344,7 +1353,7 @@
       </c>
       <c r="C12" s="15">
         <f>C8-C11</f>
-        <v>69571.319999999992</v>
+        <v>61506</v>
       </c>
       <c r="D12" s="31"/>
       <c r="G12" s="12"/>
@@ -1618,10 +1627,11 @@
         <v>20</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="D29" s="28">
-        <v>45538</v>
+        <f>+'Financial Model'!Q3</f>
+        <v>45622</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="8"/>
@@ -1694,8 +1704,8 @@
         <v>25</v>
       </c>
       <c r="C34" s="50">
-        <f>+C6/'Financial Model'!P71</f>
-        <v>28.049442198868228</v>
+        <f>+C6/'Financial Model'!Q71</f>
+        <v>23.587538226299696</v>
       </c>
       <c r="D34" s="51"/>
       <c r="G34" s="12"/>
@@ -1713,8 +1723,8 @@
         <v>26</v>
       </c>
       <c r="C35" s="50">
-        <f>+C8/SUM('Financial Model'!M7:P7)</f>
-        <v>11.954232558139534</v>
+        <f>+C8/SUM('Financial Model'!O7:Q7)</f>
+        <v>13.736642920747997</v>
       </c>
       <c r="D35" s="51"/>
       <c r="G35" s="12"/>
@@ -1732,8 +1742,8 @@
         <v>27</v>
       </c>
       <c r="C36" s="50">
-        <f>+C6/SUM('Financial Model'!M22:P22)</f>
-        <v>65.277899355462978</v>
+        <f>+C6/SUM('Financial Model'!O22:Q22)</f>
+        <v>76.434317645358632</v>
       </c>
       <c r="D36" s="51"/>
       <c r="G36" s="12"/>
@@ -1751,8 +1761,8 @@
         <v>114</v>
       </c>
       <c r="C37" s="50">
-        <f>+C6/'Financial Model'!P88</f>
-        <v>61.41090265486725</v>
+        <f>+C6/'Financial Model'!Q88</f>
+        <v>46.888297872340424</v>
       </c>
       <c r="D37" s="51"/>
       <c r="G37" s="12"/>
@@ -1846,11 +1856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962F6E9D-1442-4F5B-A570-7043CF769B1D}">
   <dimension ref="B1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
+      <selection pane="bottomRight" activeCell="S86" sqref="S86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1905,7 +1915,7 @@
       <c r="P1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="20" t="s">
         <v>128</v>
       </c>
       <c r="R1" s="17" t="s">
@@ -1983,6 +1993,9 @@
       <c r="P2" s="21">
         <v>45504</v>
       </c>
+      <c r="Q2" s="21">
+        <v>45596</v>
+      </c>
       <c r="V2" s="21">
         <v>43496</v>
       </c>
@@ -2019,6 +2032,9 @@
       <c r="P3" s="19">
         <v>45538</v>
       </c>
+      <c r="Q3" s="19">
+        <v>45622</v>
+      </c>
       <c r="X3" s="19">
         <v>44305</v>
       </c>
@@ -2076,6 +2092,9 @@
       <c r="P4" s="23">
         <v>1408</v>
       </c>
+      <c r="Q4" s="23">
+        <v>1457</v>
+      </c>
       <c r="V4" s="23">
         <v>1802.3</v>
       </c>
@@ -2144,6 +2163,9 @@
       <c r="P5" s="23">
         <v>11</v>
       </c>
+      <c r="Q5" s="23">
+        <v>9</v>
+      </c>
       <c r="V5" s="23">
         <v>635.1</v>
       </c>
@@ -2212,6 +2234,9 @@
       <c r="P6" s="23">
         <v>86</v>
       </c>
+      <c r="Q6" s="23">
+        <v>104</v>
+      </c>
       <c r="V6" s="23">
         <v>132.4</v>
       </c>
@@ -2292,12 +2317,12 @@
         <v>1505</v>
       </c>
       <c r="Q7" s="24">
-        <f>+P7*(1+Q30)</f>
-        <v>1700.6499999999999</v>
+        <f>+SUM(Q4:Q6)</f>
+        <v>1570</v>
       </c>
       <c r="R7" s="24">
         <f>+Q7*(1+R30)</f>
-        <v>1870.7149999999999</v>
+        <v>1727.0000000000002</v>
       </c>
       <c r="U7" s="24">
         <f t="shared" ref="U7:X7" si="5">+SUM(U4:U6)</f>
@@ -2329,7 +2354,7 @@
       </c>
       <c r="AB7" s="24">
         <f>+SUM(O7:R7)</f>
-        <v>6493.3649999999998</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="8" spans="2:30" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -2381,6 +2406,9 @@
       <c r="P8" s="23">
         <v>100</v>
       </c>
+      <c r="Q8" s="23">
+        <v>105</v>
+      </c>
       <c r="V8" s="23">
         <v>216</v>
       </c>
@@ -2449,6 +2477,9 @@
       <c r="P9" s="23">
         <v>18</v>
       </c>
+      <c r="Q9" s="23">
+        <v>19</v>
+      </c>
       <c r="V9" s="23">
         <v>54.4</v>
       </c>
@@ -2517,6 +2548,9 @@
       <c r="P10" s="23">
         <v>22</v>
       </c>
+      <c r="Q10" s="23">
+        <v>23</v>
+      </c>
       <c r="V10" s="23">
         <v>15.5</v>
       </c>
@@ -2596,6 +2630,10 @@
         <f>SUM(P8:P10)</f>
         <v>140</v>
       </c>
+      <c r="Q11" s="23">
+        <f>SUM(Q8:Q10)</f>
+        <v>147</v>
+      </c>
       <c r="U11" s="23">
         <f t="shared" ref="U11:X11" si="12">SUM(U8:U10)</f>
         <v>0</v>
@@ -2687,11 +2725,11 @@
       </c>
       <c r="Q12" s="24">
         <f>+Q7-Q11</f>
-        <v>1700.6499999999999</v>
+        <v>1423</v>
       </c>
       <c r="R12" s="24">
         <f>+R7-R11</f>
-        <v>1870.7149999999999</v>
+        <v>1727.0000000000002</v>
       </c>
       <c r="U12" s="24">
         <f t="shared" ref="U12:X12" si="19">+U7-U11</f>
@@ -2771,6 +2809,9 @@
       <c r="P13" s="2">
         <v>480</v>
       </c>
+      <c r="Q13" s="2">
+        <v>525</v>
+      </c>
       <c r="V13" s="23">
         <v>1183.9000000000001</v>
       </c>
@@ -2839,6 +2880,9 @@
       <c r="P14" s="2">
         <v>368</v>
       </c>
+      <c r="Q14" s="2">
+        <v>378</v>
+      </c>
       <c r="V14" s="23">
         <v>725</v>
       </c>
@@ -2907,6 +2951,9 @@
       <c r="P15" s="2">
         <v>161</v>
       </c>
+      <c r="Q15" s="2">
+        <v>161</v>
+      </c>
       <c r="V15" s="23">
         <v>340.1</v>
       </c>
@@ -2975,6 +3022,9 @@
       <c r="P16" s="2">
         <v>13</v>
       </c>
+      <c r="Q16" s="2">
+        <v>13</v>
+      </c>
       <c r="V16" s="23">
         <f>18+41.9</f>
         <v>59.9</v>
@@ -3058,11 +3108,11 @@
       </c>
       <c r="Q17" s="24">
         <f>+Q12-SUM(Q13:Q16)</f>
-        <v>1700.6499999999999</v>
+        <v>346</v>
       </c>
       <c r="R17" s="24">
         <f>+R12-SUM(R13:R16)</f>
-        <v>1870.7149999999999</v>
+        <v>1727.0000000000002</v>
       </c>
       <c r="U17" s="24">
         <f t="shared" ref="U17:X17" si="26">+U12-SUM(U13:U16)</f>
@@ -3142,7 +3192,7 @@
       <c r="P18" s="2">
         <v>9</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="52">
         <f>+AVERAGE(L18:P18)</f>
         <v>4.5999999999999996</v>
       </c>
@@ -3229,6 +3279,10 @@
         <f>+P17+P18</f>
         <v>352</v>
       </c>
+      <c r="Q19" s="23">
+        <f>+Q17+Q18</f>
+        <v>350.6</v>
+      </c>
       <c r="U19" s="23">
         <f t="shared" ref="U19:X19" si="33">+U17+U18</f>
         <v>0</v>
@@ -3307,6 +3361,9 @@
       <c r="P20" s="2">
         <v>70</v>
       </c>
+      <c r="Q20" s="52">
+        <v>76</v>
+      </c>
       <c r="V20" s="23">
         <v>38.1</v>
       </c>
@@ -3386,6 +3443,10 @@
         <f>+P19-P20</f>
         <v>282</v>
       </c>
+      <c r="Q21" s="24">
+        <f>+Q19-Q20</f>
+        <v>274.60000000000002</v>
+      </c>
       <c r="U21" s="24">
         <f t="shared" ref="U21:X21" si="40">+U19-U20</f>
         <v>0</v>
@@ -3452,7 +3513,7 @@
         <v>1.3564814814814814</v>
       </c>
       <c r="K22" s="25">
-        <f t="shared" ref="K22:P22" si="43">+K21/K23</f>
+        <f t="shared" ref="K22:Q22" si="43">+K21/K23</f>
         <v>0.74883720930232556</v>
       </c>
       <c r="L22" s="25">
@@ -3475,6 +3536,10 @@
         <f t="shared" si="43"/>
         <v>1.3055555555555556</v>
       </c>
+      <c r="Q22" s="25">
+        <f t="shared" si="43"/>
+        <v>1.2772093023255815</v>
+      </c>
       <c r="V22" s="25">
         <f t="shared" ref="V22:AA22" si="44">+V21/V23</f>
         <v>-0.36911831886706264</v>
@@ -3549,6 +3614,9 @@
       <c r="P23" s="2">
         <v>216</v>
       </c>
+      <c r="Q23" s="2">
+        <v>215</v>
+      </c>
       <c r="V23" s="23">
         <v>218.9</v>
       </c>
@@ -3628,32 +3696,33 @@
         <f t="shared" si="46"/>
         <v>0.90697674418604646</v>
       </c>
+      <c r="Q25" s="27">
+        <f t="shared" ref="Q25" si="47">+Q12/Q7</f>
+        <v>0.90636942675159238</v>
+      </c>
       <c r="V25" s="27">
-        <f t="shared" ref="V25:AA25" si="47">+V12/V7</f>
+        <f t="shared" ref="V25:AB25" si="48">+V12/V7</f>
         <v>0.88874620593042253</v>
       </c>
       <c r="W25" s="27">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.90077268423785239</v>
       </c>
       <c r="X25" s="27">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.9110647952722668</v>
       </c>
       <c r="Y25" s="27">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.90469676242590058</v>
       </c>
       <c r="Z25" s="27">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.90409590409590412</v>
       </c>
       <c r="AA25" s="27">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.90704020374749861</v>
-      </c>
-      <c r="AB25" s="27">
-        <v>9.14</v>
       </c>
     </row>
     <row r="26" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -3661,83 +3730,87 @@
         <v>56</v>
       </c>
       <c r="C26" s="27">
-        <f t="shared" ref="C26:J26" si="48">+C17/C7</f>
+        <f t="shared" ref="C26:J26" si="49">+C17/C7</f>
         <v>0.13549039433771487</v>
       </c>
       <c r="D26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.13962264150943396</v>
       </c>
       <c r="E26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.17140319715808169</v>
       </c>
       <c r="F26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.1180842279108175</v>
       </c>
       <c r="G26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.18290598290598289</v>
       </c>
       <c r="H26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.19563459983831852</v>
       </c>
       <c r="I26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.2</v>
       </c>
       <c r="J26" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.2101669195751138</v>
       </c>
       <c r="K26" s="27">
-        <f t="shared" ref="K26:P26" si="49">+K17/K7</f>
+        <f t="shared" ref="K26:P26" si="50">+K17/K7</f>
         <v>0.17100078802206461</v>
       </c>
       <c r="L26" s="27">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.19479553903345725</v>
       </c>
       <c r="M26" s="27">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.23620933521923621</v>
       </c>
       <c r="N26" s="27">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.21443158611300203</v>
       </c>
       <c r="O26" s="27">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.21100917431192662</v>
       </c>
       <c r="P26" s="27">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>0.22790697674418606</v>
       </c>
+      <c r="Q26" s="27">
+        <f t="shared" ref="Q26" si="51">+Q17/Q7</f>
+        <v>0.22038216560509555</v>
+      </c>
       <c r="V26" s="27">
-        <f t="shared" ref="V26:AA26" si="50">+V17/V7</f>
+        <f t="shared" ref="V26:AA26" si="52">+V17/V7</f>
         <v>-9.7283835317923568E-3</v>
       </c>
       <c r="W26" s="27">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0.10475521485508352</v>
       </c>
       <c r="X26" s="27">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0.16597192908400166</v>
       </c>
       <c r="Y26" s="27">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0.1409028727770178</v>
       </c>
       <c r="Z26" s="27">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0.19760239760239759</v>
       </c>
       <c r="AA26" s="27">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0.20520283791158814</v>
       </c>
     </row>
@@ -3746,83 +3819,87 @@
         <v>57</v>
       </c>
       <c r="C27" s="27">
-        <f t="shared" ref="C27:J27" si="51">+C21/C7</f>
+        <f t="shared" ref="C27:J27" si="53">+C21/C7</f>
         <v>0.15773508594539939</v>
       </c>
       <c r="D27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.10849056603773585</v>
       </c>
       <c r="E27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.1216696269982238</v>
       </c>
       <c r="F27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>7.3492981007431873E-2</v>
       </c>
       <c r="G27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.12478632478632479</v>
       </c>
       <c r="H27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.15036378334680678</v>
       </c>
       <c r="I27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.15468750000000001</v>
       </c>
       <c r="J27" s="27">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.22230652503793627</v>
       </c>
       <c r="K27" s="27">
-        <f t="shared" ref="K27:P27" si="52">+K21/K7</f>
+        <f t="shared" ref="K27:P27" si="54">+K21/K7</f>
         <v>0.12687155240346729</v>
       </c>
       <c r="L27" s="27">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.16505576208178438</v>
       </c>
       <c r="M27" s="27">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.17043847241867044</v>
       </c>
       <c r="N27" s="27">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.19196732471068753</v>
       </c>
       <c r="O27" s="27">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.17784050811573748</v>
       </c>
       <c r="P27" s="27">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.18737541528239202</v>
       </c>
+      <c r="Q27" s="27">
+        <f t="shared" ref="Q27" si="55">+Q21/Q7</f>
+        <v>0.17490445859872614</v>
+      </c>
       <c r="V27" s="27">
-        <f t="shared" ref="V27:AA27" si="53">+V21/V7</f>
+        <f t="shared" ref="V27:AA27" si="56">+V21/V7</f>
         <v>-3.1442135574752901E-2</v>
       </c>
       <c r="W27" s="27">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>6.5510185383135328E-2</v>
       </c>
       <c r="X27" s="27">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.31875263824398475</v>
       </c>
       <c r="Y27" s="27">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.11331509347925217</v>
       </c>
       <c r="Z27" s="27">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.16443556443556442</v>
       </c>
       <c r="AA27" s="27">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.16481717300345644</v>
       </c>
     </row>
@@ -3831,83 +3908,87 @@
         <v>58</v>
       </c>
       <c r="C28" s="27">
-        <f t="shared" ref="C28:J28" si="54">+C20/C19</f>
+        <f t="shared" ref="C28:J28" si="57">+C20/C19</f>
         <v>-0.19083969465648856</v>
       </c>
       <c r="D28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.17266187050359713</v>
       </c>
       <c r="E28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.27127659574468083</v>
       </c>
       <c r="F28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.16822429906542055</v>
       </c>
       <c r="G28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.25128205128205128</v>
       </c>
       <c r="H28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.19827586206896552</v>
       </c>
       <c r="I28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="J28" s="27">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>-5.7761732851985562E-2</v>
       </c>
       <c r="K28" s="27">
-        <f t="shared" ref="K28:P28" si="55">+K20/K19</f>
+        <f t="shared" ref="K28:P28" si="58">+K20/K19</f>
         <v>0.27149321266968324</v>
       </c>
       <c r="L28" s="27">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.13953488372093023</v>
       </c>
       <c r="M28" s="27">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.24687500000000001</v>
       </c>
       <c r="N28" s="27">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.16320474777448071</v>
       </c>
       <c r="O28" s="27">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.18446601941747573</v>
       </c>
       <c r="P28" s="27">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.19886363636363635</v>
       </c>
+      <c r="Q28" s="27">
+        <f t="shared" ref="Q28" si="59">+Q20/Q19</f>
+        <v>0.21677124928693667</v>
+      </c>
       <c r="V28" s="27">
-        <f t="shared" ref="V28:AA28" si="56">+V20/V19</f>
+        <f t="shared" ref="V28:AA28" si="60">+V20/V19</f>
         <v>-0.89227166276346603</v>
       </c>
       <c r="W28" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.27238805970149249</v>
       </c>
       <c r="X28" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>-1.2099871959026891</v>
       </c>
       <c r="Y28" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.12035398230088495</v>
       </c>
       <c r="Z28" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.13002114164904863</v>
       </c>
       <c r="AA28" s="27">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.20246478873239437</v>
       </c>
     </row>
@@ -3928,74 +4009,75 @@
         <v>129</v>
       </c>
       <c r="G30" s="26">
-        <f t="shared" ref="G30:P30" si="57">+G7/C7-1</f>
+        <f t="shared" ref="G30:Q30" si="61">+G7/C7-1</f>
         <v>0.18301314459049545</v>
       </c>
       <c r="H30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.16698113207547172</v>
       </c>
       <c r="I30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.13676731793960917</v>
       </c>
       <c r="J30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>8.8356729975227033E-2</v>
       </c>
       <c r="K30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>8.4615384615384537E-2</v>
       </c>
       <c r="L30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>8.730800323362975E-2</v>
       </c>
       <c r="M30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.10468750000000004</v>
       </c>
       <c r="N30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.11456752655538693</v>
       </c>
       <c r="O30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.11662726556343572</v>
       </c>
       <c r="P30" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0.11895910780669139</v>
       </c>
       <c r="Q30" s="26">
-        <v>0.13</v>
+        <f t="shared" si="61"/>
+        <v>0.11032531824611036</v>
       </c>
       <c r="R30" s="26">
         <v>0.1</v>
       </c>
       <c r="W30" s="26">
-        <f>+W7/V7-1</f>
+        <f t="shared" ref="W30:AB30" si="62">+W7/V7-1</f>
         <v>0.27414584792590868</v>
       </c>
       <c r="X30" s="26">
-        <f>+X7/W7-1</f>
+        <f t="shared" si="62"/>
         <v>0.15762147634608925</v>
       </c>
       <c r="Y30" s="26">
-        <f>+Y7/X7-1</f>
+        <f t="shared" si="62"/>
         <v>0.15713381173490926</v>
       </c>
       <c r="Z30" s="26">
-        <f>+Z7/Y7-1</f>
+        <f t="shared" si="62"/>
         <v>0.14113087095303234</v>
       </c>
       <c r="AA30" s="26">
-        <f>+AA7/Z7-1</f>
+        <f t="shared" si="62"/>
         <v>9.8301698301698215E-2</v>
       </c>
       <c r="AB30" s="26">
-        <f>+AB7/AA7-1</f>
-        <v>0.18125613971257049</v>
+        <f t="shared" si="62"/>
+        <v>0.13134436965617602</v>
       </c>
     </row>
     <row r="31" spans="2:28" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -4006,63 +4088,63 @@
         <v>129</v>
       </c>
       <c r="D31" s="27">
-        <f t="shared" ref="D31:R31" si="58">+D7/C7-1</f>
+        <f t="shared" ref="D31:R31" si="63">+D7/C7-1</f>
         <v>7.1789686552072851E-2</v>
       </c>
       <c r="E31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>6.2264150943396324E-2</v>
       </c>
       <c r="F31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>7.5488454706927222E-2</v>
       </c>
       <c r="G31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>-3.3856317093311272E-2</v>
       </c>
       <c r="H31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>5.7264957264957284E-2</v>
       </c>
       <c r="I31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>3.4761519805982299E-2</v>
       </c>
       <c r="J31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>2.9687500000000089E-2</v>
       </c>
       <c r="K31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>-3.7177541729893737E-2</v>
       </c>
       <c r="L31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>5.9889676910953593E-2</v>
       </c>
       <c r="M31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>5.1301115241635609E-2</v>
       </c>
       <c r="N31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>3.8896746817538963E-2</v>
       </c>
       <c r="O31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>-3.539823008849563E-2</v>
       </c>
       <c r="P31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>6.2103034580098804E-2</v>
       </c>
       <c r="Q31" s="27">
-        <f t="shared" si="58"/>
-        <v>0.12999999999999989</v>
+        <f t="shared" si="63"/>
+        <v>4.3189368770764069E-2</v>
       </c>
       <c r="R31" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="U31" s="34" t="s">
@@ -4090,12 +4172,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="2:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="24" t="s">
         <v>6</v>
       </c>
@@ -4105,8 +4187,11 @@
       <c r="P38" s="24">
         <v>1513</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q38" s="24">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="24" t="s">
         <v>62</v>
       </c>
@@ -4116,8 +4201,11 @@
       <c r="P39" s="24">
         <v>365</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q39" s="24">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="23" t="s">
         <v>63</v>
       </c>
@@ -4127,8 +4215,11 @@
       <c r="P40" s="23">
         <v>402</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q40" s="23">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="23" t="s">
         <v>64</v>
       </c>
@@ -4138,69 +4229,76 @@
       <c r="P41" s="23">
         <v>478</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q41" s="23">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="23" t="s">
         <v>65</v>
       </c>
       <c r="C42" s="23">
-        <f t="shared" ref="C42:F42" si="59">+SUM(C38:C41)</f>
+        <f t="shared" ref="C42:F42" si="64">+SUM(C38:C41)</f>
         <v>0</v>
       </c>
       <c r="D42" s="23">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="E42" s="23">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="F42" s="23">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="G42" s="23">
-        <f t="shared" ref="G42:O42" si="60">+SUM(G38:G41)</f>
+        <f t="shared" ref="G42:O42" si="65">+SUM(G38:G41)</f>
         <v>0</v>
       </c>
       <c r="H42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="I42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="J42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="K42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="L42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="M42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="N42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O42" s="23">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>2810</v>
       </c>
       <c r="P42" s="23">
         <f>+SUM(P38:P41)</f>
         <v>2758</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q42" s="23">
+        <f>+SUM(Q38:Q41)</f>
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="24" t="s">
         <v>66</v>
       </c>
@@ -4210,8 +4308,11 @@
       <c r="P43" s="24">
         <v>231</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q43" s="24">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="23" t="s">
         <v>68</v>
       </c>
@@ -4221,8 +4322,11 @@
       <c r="P44" s="23">
         <v>116</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q44" s="23">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="23" t="s">
         <v>67</v>
       </c>
@@ -4232,8 +4336,11 @@
       <c r="P45" s="23">
         <v>205</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q45" s="23">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="23" t="s">
         <v>69</v>
       </c>
@@ -4245,8 +4352,12 @@
         <f>609+4253</f>
         <v>4862</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q46" s="23">
+        <f>594+4256</f>
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="23" t="s">
         <v>70</v>
       </c>
@@ -4256,8 +4367,11 @@
       <c r="P47" s="23">
         <v>1129</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q47" s="23">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B48" s="23" t="s">
         <v>71</v>
       </c>
@@ -4267,70 +4381,77 @@
       <c r="P48" s="23">
         <v>659</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q48" s="23">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B49" s="23" t="s">
         <v>72</v>
       </c>
       <c r="C49" s="23">
-        <f t="shared" ref="C49:F49" si="61">+SUM(C42:C48)</f>
+        <f t="shared" ref="C49:F49" si="66">+SUM(C42:C48)</f>
         <v>0</v>
       </c>
       <c r="D49" s="23">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="E49" s="23">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="F49" s="23">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="G49" s="23">
-        <f t="shared" ref="G49:O49" si="62">+SUM(G42:G48)</f>
+        <f t="shared" ref="G49:O49" si="67">+SUM(G42:G48)</f>
         <v>0</v>
       </c>
       <c r="H49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="I49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="J49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="K49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="L49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="M49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="N49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O49" s="23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>9830</v>
       </c>
       <c r="P49" s="23">
         <f>+SUM(P42:P48)</f>
         <v>9960</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q49" s="23">
+        <f>+SUM(Q42:Q48)</f>
+        <v>10133</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="23" t="s">
         <v>73</v>
       </c>
@@ -4340,8 +4461,11 @@
       <c r="P51" s="23">
         <v>174</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q51" s="23">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="23" t="s">
         <v>74</v>
       </c>
@@ -4351,8 +4475,11 @@
       <c r="P52" s="23">
         <v>361</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q52" s="23">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="23" t="s">
         <v>75</v>
       </c>
@@ -4362,8 +4489,11 @@
       <c r="P53" s="23">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q53" s="23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="23" t="s">
         <v>76</v>
       </c>
@@ -4373,8 +4503,11 @@
       <c r="P54" s="23">
         <v>3228</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q54" s="23">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="23" t="s">
         <v>77</v>
       </c>
@@ -4384,8 +4517,11 @@
       <c r="P55" s="23">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q55" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="24" t="s">
         <v>80</v>
       </c>
@@ -4395,8 +4531,11 @@
       <c r="P56" s="24">
         <v>300</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q56" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="23" t="s">
         <v>78</v>
       </c>
@@ -4406,69 +4545,76 @@
       <c r="P57" s="23">
         <v>159</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q57" s="23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="23" t="s">
         <v>79</v>
       </c>
       <c r="C58" s="23">
-        <f t="shared" ref="C58:F58" si="63">+SUM(C51:C57)</f>
+        <f t="shared" ref="C58:F58" si="68">+SUM(C51:C57)</f>
         <v>0</v>
       </c>
       <c r="D58" s="23">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="E58" s="23">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="F58" s="23">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="G58" s="23">
-        <f t="shared" ref="G58:O58" si="64">+SUM(G51:G57)</f>
+        <f t="shared" ref="G58:O58" si="69">+SUM(G51:G57)</f>
         <v>0</v>
       </c>
       <c r="H58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="I58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="J58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="K58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="L58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="M58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="N58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="O58" s="23">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>4097</v>
       </c>
       <c r="P58" s="23">
         <f>+SUM(P51:P57)</f>
         <v>4337</v>
       </c>
-    </row>
-    <row r="59" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q58" s="23">
+        <f>+SUM(Q51:Q57)</f>
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="23" t="s">
         <v>81</v>
       </c>
@@ -4478,8 +4624,11 @@
       <c r="P59" s="23">
         <v>464</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q59" s="23">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="23" t="s">
         <v>82</v>
       </c>
@@ -4489,8 +4638,11 @@
       <c r="P60" s="23">
         <v>250</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q60" s="23">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="23" t="s">
         <v>83</v>
       </c>
@@ -4500,8 +4652,11 @@
       <c r="P61" s="23">
         <v>183</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q61" s="23">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="23" t="s">
         <v>89</v>
       </c>
@@ -4511,8 +4666,11 @@
       <c r="P62" s="23">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="2:16" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q62" s="23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="24" t="s">
         <v>84</v>
       </c>
@@ -4522,8 +4680,11 @@
       <c r="P63" s="24">
         <v>1986</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q63" s="24">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="23" t="s">
         <v>85</v>
       </c>
@@ -4533,70 +4694,77 @@
       <c r="P64" s="23">
         <v>230</v>
       </c>
-    </row>
-    <row r="65" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q64" s="23">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C65" s="23">
-        <f t="shared" ref="C65:F65" si="65">+SUM(C58:C64)</f>
+        <f t="shared" ref="C65:F65" si="70">+SUM(C58:C64)</f>
         <v>0</v>
       </c>
       <c r="D65" s="23">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="E65" s="23">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="F65" s="23">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="G65" s="23">
-        <f t="shared" ref="G65:O65" si="66">+SUM(G58:G64)</f>
+        <f t="shared" ref="G65:O65" si="71">+SUM(G58:G64)</f>
         <v>0</v>
       </c>
       <c r="H65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="I65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="J65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="K65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="L65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="M65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="N65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="O65" s="23">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>7669</v>
       </c>
       <c r="P65" s="23">
         <f>+SUM(P58:P64)</f>
         <v>7486</v>
       </c>
-    </row>
-    <row r="66" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q65" s="23">
+        <f>+SUM(Q58:Q64)</f>
+        <v>7517</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="23" t="s">
         <v>87</v>
       </c>
@@ -4606,8 +4774,11 @@
       <c r="P67" s="23">
         <v>2474</v>
       </c>
-    </row>
-    <row r="68" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q67" s="23">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="23" t="s">
         <v>88</v>
       </c>
@@ -4619,73 +4790,97 @@
         <f>+P67+P65</f>
         <v>9960</v>
       </c>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q68" s="23">
+        <f>+Q67+Q65</f>
+        <v>10133</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>90</v>
       </c>
       <c r="O70" s="23">
-        <f t="shared" ref="O70" si="67">+O49-O65</f>
+        <f t="shared" ref="O70" si="72">+O49-O65</f>
         <v>2161</v>
       </c>
       <c r="P70" s="23">
         <f>+P49-P65</f>
         <v>2474</v>
       </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q70" s="23">
+        <f>+Q49-Q65</f>
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
         <v>91</v>
       </c>
       <c r="O71" s="2">
-        <f t="shared" ref="O71" si="68">+O70/O23</f>
+        <f t="shared" ref="O71" si="73">+O70/O23</f>
         <v>10.051162790697674</v>
       </c>
       <c r="P71" s="2">
         <f>+P70/P23</f>
         <v>11.453703703703704</v>
       </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q71" s="2">
+        <f>+Q70/Q23</f>
+        <v>12.167441860465116</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O73" s="23">
-        <f t="shared" ref="O73" si="69">+O38+O39+O43</f>
+        <f t="shared" ref="O73" si="74">+O38+O39+O43</f>
         <v>2227</v>
       </c>
       <c r="P73" s="23">
         <f>+P38+P39+P43</f>
         <v>2109</v>
       </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q73" s="23">
+        <f>+Q38+Q39+Q43</f>
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>7</v>
       </c>
       <c r="O74" s="23">
-        <f t="shared" ref="O74" si="70">+O56+O63</f>
+        <f t="shared" ref="O74" si="75">+O56+O63</f>
         <v>2285</v>
       </c>
       <c r="P74" s="23">
         <f>+P56+P63</f>
         <v>2286</v>
       </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q74" s="23">
+        <f>+Q56+Q63</f>
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>8</v>
       </c>
       <c r="O75" s="23">
-        <f t="shared" ref="O75" si="71">+O73-O74</f>
+        <f t="shared" ref="O75" si="76">+O73-O74</f>
         <v>-58</v>
       </c>
       <c r="P75" s="23">
         <f>+P73-P74</f>
         <v>-177</v>
       </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q75" s="23">
+        <f>+Q73-Q74</f>
+        <v>-309</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>113</v>
       </c>
@@ -4701,8 +4896,11 @@
       <c r="P77" s="2">
         <v>247.52</v>
       </c>
-    </row>
-    <row r="78" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q77" s="2">
+        <v>283.8</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="23" t="s">
         <v>5</v>
       </c>
@@ -4722,8 +4920,12 @@
         <f>+P77*P23</f>
         <v>53464.32</v>
       </c>
-    </row>
-    <row r="79" spans="2:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q78" s="23">
+        <f>+Q77*Q23</f>
+        <v>61017</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="23" t="s">
         <v>9</v>
       </c>
@@ -4735,6 +4937,10 @@
         <f>+P78-P75</f>
         <v>53641.32</v>
       </c>
+      <c r="Q79" s="23">
+        <f>+Q78-Q75</f>
+        <v>61326</v>
+      </c>
     </row>
     <row r="82" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B82" s="29" t="s">
@@ -4797,6 +5003,10 @@
         <f>706-O83</f>
         <v>212</v>
       </c>
+      <c r="Q83" s="23">
+        <f>915-SUM(O83:P83)</f>
+        <v>209</v>
+      </c>
       <c r="V83" s="23">
         <v>377.1</v>
       </c>
@@ -4872,6 +5082,10 @@
         <f>16-O84</f>
         <v>9</v>
       </c>
+      <c r="Q84" s="2">
+        <f>26-SUM(O84:P84)</f>
+        <v>10</v>
+      </c>
       <c r="V84" s="2">
         <v>67</v>
       </c>
@@ -4896,71 +5110,75 @@
         <v>95</v>
       </c>
       <c r="C85" s="23">
-        <f t="shared" ref="C85:P85" si="72">+C83-C84</f>
+        <f t="shared" ref="C85:Q85" si="77">+C83-C84</f>
         <v>316</v>
       </c>
       <c r="D85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>186</v>
       </c>
       <c r="E85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>275</v>
       </c>
       <c r="F85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>698</v>
       </c>
       <c r="G85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>422</v>
       </c>
       <c r="H85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>246</v>
       </c>
       <c r="I85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>460</v>
       </c>
       <c r="J85" s="23">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>903</v>
       </c>
       <c r="K85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>714</v>
       </c>
       <c r="L85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>128</v>
       </c>
       <c r="M85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>13</v>
       </c>
       <c r="N85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>427</v>
       </c>
       <c r="O85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>487</v>
       </c>
       <c r="P85" s="2">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>203</v>
+      </c>
+      <c r="Q85" s="2">
+        <f t="shared" si="77"/>
+        <v>199</v>
       </c>
       <c r="V85" s="23">
         <f>+V83-V84</f>
         <v>310.10000000000002</v>
       </c>
       <c r="W85" s="23">
-        <f t="shared" ref="W85:X85" si="73">+W83-W84</f>
+        <f t="shared" ref="W85:X85" si="78">+W83-W84</f>
         <v>1361.8999999999999</v>
       </c>
       <c r="X85" s="23">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>1346.1000000000001</v>
       </c>
       <c r="Y85" s="23">
@@ -4992,28 +5210,32 @@
         <f>+SUM(M85:P85)</f>
         <v>1130</v>
       </c>
+      <c r="Q87" s="23">
+        <f>+SUM(N85:Q85)</f>
+        <v>1316</v>
+      </c>
       <c r="V87" s="23">
-        <f t="shared" ref="V87:AA87" si="74">+V85</f>
+        <f t="shared" ref="V87:AA87" si="79">+V85</f>
         <v>310.10000000000002</v>
       </c>
       <c r="W87" s="23">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>1361.8999999999999</v>
       </c>
       <c r="X87" s="23">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>1346.1000000000001</v>
       </c>
       <c r="Y87" s="23">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>1475</v>
       </c>
       <c r="Z87" s="23">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>2031</v>
       </c>
       <c r="AA87" s="23">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>1282</v>
       </c>
     </row>
@@ -5033,28 +5255,32 @@
         <f>+P87/P23</f>
         <v>5.2314814814814818</v>
       </c>
+      <c r="Q88" s="38">
+        <f>+Q87/Q23</f>
+        <v>6.1209302325581394</v>
+      </c>
       <c r="V88" s="38">
-        <f t="shared" ref="V88:AA88" si="75">+V87/V23</f>
+        <f t="shared" ref="V88:AA88" si="80">+V87/V23</f>
         <v>1.4166285975331203</v>
       </c>
       <c r="W88" s="38">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>6.1989076012744651</v>
       </c>
       <c r="X88" s="38">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>6.135369188696445</v>
       </c>
       <c r="Y88" s="38">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>6.7045454545454541</v>
       </c>
       <c r="Z88" s="38">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>9.4027777777777786</v>
       </c>
       <c r="AA88" s="38">
-        <f t="shared" si="75"/>
+        <f t="shared" si="80"/>
         <v>5.990654205607477</v>
       </c>
     </row>
@@ -5073,6 +5299,10 @@
       <c r="P89" s="32">
         <f>+P77/P88</f>
         <v>47.313557522123894</v>
+      </c>
+      <c r="Q89" s="32">
+        <f>+Q77/Q88</f>
+        <v>46.36550151975684</v>
       </c>
     </row>
   </sheetData>
@@ -5085,13 +5315,14 @@
     <hyperlink ref="I1" r:id="rId5" xr:uid="{B478A006-1CD0-4FE4-8592-310B443EAD69}"/>
     <hyperlink ref="H1" r:id="rId6" xr:uid="{F83179AB-C30C-4A94-9151-352BC85A87C1}"/>
     <hyperlink ref="G1" r:id="rId7" xr:uid="{A7372BD3-E118-41F5-956D-A3C8C84541EC}"/>
+    <hyperlink ref="Q1" r:id="rId8" xr:uid="{DAC10289-E8E7-4B79-A354-7C48FC0680CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <ignoredErrors>
-    <ignoredError sqref="O7:P7 M7 I7 X7 X11:X12 X17 X19 X21 X24" formulaRange="1"/>
+    <ignoredError sqref="O7:Q7 M7 I7 X7 X11:X12 X17 X19 X21 X24" formulaRange="1"/>
     <ignoredError sqref="N7:N22 J7:J23 F7:F23" formula="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>